<commit_message>
updated results, report and bench
</commit_message>
<xml_diff>
--- a/src/testbench.xlsx
+++ b/src/testbench.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Semester_project_git\2022-msc-sem-proj-nseemann\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB3F61FC-A1F7-404C-894F-4C8E8BD91061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8973E8-4B0A-448D-B29B-DB55F84E27D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{5F350800-DD2F-4C68-9341-F5452F06AE8A}"/>
+    <workbookView xWindow="-12" yWindow="-12" windowWidth="23064" windowHeight="6120" xr2:uid="{5F350800-DD2F-4C68-9341-F5452F06AE8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="78">
   <si>
     <t>default params</t>
   </si>
@@ -120,15 +122,6 @@
     <t>added_skips</t>
   </si>
   <si>
-    <t>4 vehicles max, 1 or 2 set_add_skips, all divided by 1000</t>
-  </si>
-  <si>
-    <t>3 vehicles max, 1 set_add_skips, all divided by 1000</t>
-  </si>
-  <si>
-    <t>3 vehicles max, 2 set_add_skips, all divided by 1000</t>
-  </si>
-  <si>
     <t>22-12-01_10-50_output</t>
   </si>
   <si>
@@ -151,12 +144,142 @@
   </si>
   <si>
     <t>Max added scens</t>
+  </si>
+  <si>
+    <t>3 vehicles max, 2 set_add_skips, all divided by 1000, confirmed at per week consider 3</t>
+  </si>
+  <si>
+    <t>3 vehicles max, 1 set_add_skips, all divided by 1000, per week consider 3</t>
+  </si>
+  <si>
+    <t>3 vehicles max, 2 set_add_skips, all divided by 1000, ambiguous per week consider</t>
+  </si>
+  <si>
+    <t>22-12-01_15-021_output</t>
+  </si>
+  <si>
+    <t>22-12-01_15-062_output</t>
+  </si>
+  <si>
+    <t>22-12-01_16-073_output</t>
+  </si>
+  <si>
+    <t>22-12-01_17-194_output</t>
+  </si>
+  <si>
+    <t>22-12-01_19-105_output</t>
+  </si>
+  <si>
+    <t>22-12-01_19-266_output</t>
+  </si>
+  <si>
+    <t>22-12-02_05-347_output</t>
+  </si>
+  <si>
+    <t>22-12-02_05-388_output</t>
+  </si>
+  <si>
+    <t>22-12-02_05-449_output</t>
+  </si>
+  <si>
+    <t>22-12-02_06-0810_output</t>
+  </si>
+  <si>
+    <t>4 vehicles max, 1, all divided by 1000, per week consider 3</t>
+  </si>
+  <si>
+    <t>4 vehicles max, 1, all divided by 1000, per week consider ambiguous</t>
+  </si>
+  <si>
+    <t>22-12-02_08-081_output</t>
+  </si>
+  <si>
+    <t>22-12-02_07-022_output</t>
+  </si>
+  <si>
+    <t>22-12-02_07-043_output</t>
+  </si>
+  <si>
+    <t>22-12-02_07-064_output</t>
+  </si>
+  <si>
+    <t>22-12-02_07-095_output</t>
+  </si>
+  <si>
+    <t>22-12-02_07-126_output</t>
+  </si>
+  <si>
+    <t>22-12-02_07-167_output</t>
+  </si>
+  <si>
+    <t>22-12-02_07-348_output</t>
+  </si>
+  <si>
+    <t>22-12-02_07-529_output</t>
+  </si>
+  <si>
+    <t>22-12-02_07-5810_output</t>
+  </si>
+  <si>
+    <t>22-12-02_07-001_output</t>
+  </si>
+  <si>
+    <t>SA1 3V</t>
+  </si>
+  <si>
+    <t>SA2 3V</t>
+  </si>
+  <si>
+    <t>max_add_skips</t>
+  </si>
+  <si>
+    <t>delta price</t>
+  </si>
+  <si>
+    <t>added_skip</t>
+  </si>
+  <si>
+    <t>distance from dump</t>
+  </si>
+  <si>
+    <t>filling rate</t>
+  </si>
+  <si>
+    <t>18,33,35,42,44</t>
+  </si>
+  <si>
+    <t>1,0.5,0.5,1,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8.3,17.1, 15.7,13.3,11.9</t>
+  </si>
+  <si>
+    <t>18,42,42,44</t>
+  </si>
+  <si>
+    <t>1,1,1,1</t>
+  </si>
+  <si>
+    <t>8.3,13.3,13.3,11.9</t>
+  </si>
+  <si>
+    <t>-42 +32,33</t>
+  </si>
+  <si>
+    <t>0.5, 0.5</t>
+  </si>
+  <si>
+    <t>17.7,17.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="170" formatCode="0.0000E+00"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -266,31 +389,65 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,6 +487,7 @@
       <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -356,16 +514,40 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$D$7:$D$14</c:f>
+              <c:f>Sheet1!$D$9:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$18:$G$25</c:f>
+              <c:f>Sheet1!$G$9:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="8"/>
@@ -398,7 +580,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F71A-4F14-B38F-8A9FDC093A0A}"/>
+              <c16:uniqueId val="{00000000-3EF6-433C-9461-AC7DA78E0111}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -421,16 +603,40 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$D$7:$D$14</c:f>
+              <c:f>Sheet1!$D$9:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$18:$I$25</c:f>
+              <c:f>Sheet1!$I$9:$I$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="8"/>
@@ -463,7 +669,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F71A-4F14-B38F-8A9FDC093A0A}"/>
+              <c16:uniqueId val="{00000001-3EF6-433C-9461-AC7DA78E0111}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -486,18 +692,42 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$D$7:$D$14</c:f>
+              <c:f>Sheet1!$D$9:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$28:$G$35</c:f>
+              <c:f>Sheet1!$G$19:$G$26</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
+                <c:formatCode>0.0000E+00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1389.5306172324099</c:v>
@@ -509,26 +739,26 @@
                   <c:v>1367.3347238400002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1358.179536184</c:v>
+                  <c:v>1358.17953792</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1349.25898361341</c:v>
+                  <c:v>1349.2589913600002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1342.859153914</c:v>
+                  <c:v>1342.8591676718199</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1336.94860451</c:v>
+                  <c:v>1336.9486079999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1332.2367400000001</c:v>
+                  <c:v>1332.2367284010299</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000F-F71A-4F14-B38F-8A9FDC093A0A}"/>
+              <c16:uniqueId val="{00000002-3EF6-433C-9461-AC7DA78E0111}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -536,7 +766,7 @@
           <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
-            <c:v>bound 2</c:v>
+            <c:v>series5</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -549,16 +779,40 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$D$7:$D$14</c:f>
+              <c:f>Sheet1!$D$9:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$28:$I$35</c:f>
+              <c:f>Sheet1!$I$19:$I$26</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="8"/>
@@ -569,29 +823,29 @@
                   <c:v>1364.7559709246907</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1344.0911173088643</c:v>
+                  <c:v>1337.5254184829212</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1355.2893301310005</c:v>
+                  <c:v>1346.696372088519</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1339.503143421384</c:v>
+                  <c:v>1333.6378279747109</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1331.9229089645244</c:v>
+                  <c:v>1129.6019320129194</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1331.5069408157483</c:v>
+                  <c:v>1122.8084550564704</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1250.7735518788072</c:v>
+                  <c:v>1225.241153032696</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000010-F71A-4F14-B38F-8A9FDC093A0A}"/>
+              <c16:uniqueId val="{00000003-3EF6-433C-9461-AC7DA78E0111}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -625,20 +879,56 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4472C4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="4472C4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$D$7:$D$14</c:f>
+              <c:f>Sheet1!$D$19:$D$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$18:$G$25</c:f>
+              <c:f>Sheet1!$G$9:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="8"/>
@@ -672,7 +962,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-F71A-4F14-B38F-8A9FDC093A0A}"/>
+              <c16:uniqueId val="{00000004-3EF6-433C-9461-AC7DA78E0111}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -692,22 +982,58 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$D$7:$D$14</c:f>
+              <c:f>Sheet1!$D$19:$D$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$28:$G$35</c:f>
+              <c:f>Sheet1!$G$19:$G$26</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
+                <c:formatCode>0.0000E+00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1389.5306172324099</c:v>
@@ -719,19 +1045,19 @@
                   <c:v>1367.3347238400002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1358.179536184</c:v>
+                  <c:v>1358.17953792</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1349.25898361341</c:v>
+                  <c:v>1349.2589913600002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1342.859153914</c:v>
+                  <c:v>1342.8591676718199</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1336.94860451</c:v>
+                  <c:v>1336.9486079999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1332.2367400000001</c:v>
+                  <c:v>1332.2367284010299</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -739,7 +1065,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000012-F71A-4F14-B38F-8A9FDC093A0A}"/>
+              <c16:uniqueId val="{00000005-3EF6-433C-9461-AC7DA78E0111}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -747,14 +1073,14 @@
           <c:idx val="6"/>
           <c:order val="6"/>
           <c:tx>
-            <c:v>line1360</c:v>
+            <c:v>1320</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="6350" cap="rnd">
+            <a:ln w="9525" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="bg2">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
+                <a:srgbClr val="E7E6E6">
+                  <a:lumMod val="90000"/>
+                </a:srgbClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -765,17 +1091,41 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$U$16:$U$25</c:f>
+              <c:f>Sheet1!$N$9:$N$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1320</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1320</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1320</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1320</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1320</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1320</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1320</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1320</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000021-58BA-44B0-9D24-2C0ED2962E28}"/>
+              <c16:uniqueId val="{00000024-3EF6-433C-9461-AC7DA78E0111}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -783,14 +1133,14 @@
           <c:idx val="7"/>
           <c:order val="7"/>
           <c:tx>
-            <c:v>line1380</c:v>
+            <c:v>1340</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="6350" cap="rnd">
+            <a:ln w="9525" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="bg2">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
+                <a:srgbClr val="E7E6E6">
+                  <a:lumMod val="90000"/>
+                </a:srgbClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -801,17 +1151,41 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$28:$P$35</c:f>
+              <c:f>Sheet1!$O$9:$O$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1340</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1340</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1340</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1340</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1340</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1340</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1340</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1340</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000022-58BA-44B0-9D24-2C0ED2962E28}"/>
+              <c16:uniqueId val="{00000025-3EF6-433C-9461-AC7DA78E0111}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -819,14 +1193,14 @@
           <c:idx val="8"/>
           <c:order val="8"/>
           <c:tx>
-            <c:v>line1400</c:v>
+            <c:v>1360</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="6350" cap="rnd">
+            <a:ln w="9525" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="bg2">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
+                <a:srgbClr val="E7E6E6">
+                  <a:lumMod val="90000"/>
+                </a:srgbClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -837,17 +1211,41 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$28:$Q$35</c:f>
+              <c:f>Sheet1!$P$9:$P$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1360</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1360</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1360</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1360</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1360</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1360</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1360</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1360</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000023-58BA-44B0-9D24-2C0ED2962E28}"/>
+              <c16:uniqueId val="{00000026-3EF6-433C-9461-AC7DA78E0111}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -855,14 +1253,14 @@
           <c:idx val="9"/>
           <c:order val="9"/>
           <c:tx>
-            <c:v>line1320</c:v>
+            <c:v>1380</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="6350" cap="rnd">
+            <a:ln w="9525" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="bg2">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
+                <a:srgbClr val="E7E6E6">
+                  <a:lumMod val="90000"/>
+                </a:srgbClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -873,17 +1271,41 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$S$16:$S$25</c:f>
+              <c:f>Sheet1!$Q$9:$Q$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1380</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1380</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1380</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1380</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1380</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1380</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1380</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1380</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000024-58BA-44B0-9D24-2C0ED2962E28}"/>
+              <c16:uniqueId val="{00000027-3EF6-433C-9461-AC7DA78E0111}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -891,14 +1313,14 @@
           <c:idx val="10"/>
           <c:order val="10"/>
           <c:tx>
-            <c:v>line1340</c:v>
+            <c:v>1400</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="6350" cap="rnd">
+            <a:ln w="9525" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="bg2">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
+                <a:srgbClr val="E7E6E6">
+                  <a:lumMod val="90000"/>
+                </a:srgbClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -909,17 +1331,41 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$16:$T$25</c:f>
+              <c:f>Sheet1!$R$9:$R$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1400</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000025-58BA-44B0-9D24-2C0ED2962E28}"/>
+              <c16:uniqueId val="{00000028-3EF6-433C-9461-AC7DA78E0111}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1046,6 +1492,7 @@
         <c:axId val="212876736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1400"/>
           <c:min val="1300"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1125,7 +1572,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="0"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="0"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1806,27 +2253,29 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>337366</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>169846</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1142999</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>141514</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>502648</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>96429</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>437424</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>68097</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8ACCC2EF-6E5F-4483-807B-98060B688D74}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{777D7E4F-7744-418F-8E74-5C43E3E7D2AC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2140,10 +2589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82F78E04-2C07-4460-BA33-A46D4195128A}">
-  <dimension ref="A1:R44"/>
+  <dimension ref="A1:R38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N35" sqref="N35"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2153,12 +2602,14 @@
     <col min="7" max="7" width="16.6640625" customWidth="1"/>
     <col min="9" max="9" width="10.6640625" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="12" max="12" width="21" customWidth="1"/>
-    <col min="13" max="13" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5546875" customWidth="1"/>
-    <col min="17" max="17" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.6640625" customWidth="1"/>
+    <col min="11" max="11" width="18.88671875" customWidth="1"/>
+    <col min="12" max="12" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21" customWidth="1"/>
+    <col min="14" max="14" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5546875" customWidth="1"/>
+    <col min="18" max="18" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
@@ -2193,10 +2644,10 @@
         <v>27</v>
       </c>
       <c r="K1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" t="s">
         <v>26</v>
-      </c>
-      <c r="L1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
@@ -2284,996 +2735,2279 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
+    <row r="7" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="Q7" s="1"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="G8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
+      <c r="A8" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="2">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2">
+        <v>4</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="10"/>
+      <c r="M8">
+        <v>4</v>
+      </c>
+      <c r="N8" s="9">
+        <v>1320</v>
+      </c>
+      <c r="O8" s="28">
+        <v>1340</v>
+      </c>
+      <c r="P8">
+        <v>1360</v>
+      </c>
+      <c r="Q8">
+        <v>1380</v>
+      </c>
+      <c r="R8">
+        <v>1400</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="G9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="3">
+        <v>3</v>
+      </c>
+      <c r="D9" s="3">
+        <v>5</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1</v>
+      </c>
+      <c r="G9" s="4">
+        <v>1391.2992307200002</v>
+      </c>
+      <c r="H9" s="3">
+        <v>5.1395017022160001E-3</v>
+      </c>
+      <c r="I9" s="4">
+        <f>G9-G9*(H9)</f>
+        <v>1384.148645955423</v>
+      </c>
+      <c r="J9" s="3">
+        <v>5</v>
+      </c>
+      <c r="K9" s="25">
+        <v>17</v>
+      </c>
+      <c r="L9" s="5">
+        <f>G9-I9</f>
+        <v>7.150584764577161</v>
+      </c>
+      <c r="M9">
+        <v>5</v>
+      </c>
+      <c r="N9" s="9">
+        <v>1320</v>
+      </c>
+      <c r="O9" s="28">
+        <v>1340</v>
+      </c>
+      <c r="P9">
+        <v>1360</v>
+      </c>
+      <c r="Q9">
+        <v>1380</v>
+      </c>
+      <c r="R9">
+        <v>1400</v>
+      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="G10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="3">
+        <v>3</v>
+      </c>
+      <c r="D10" s="3">
+        <v>6</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3">
+        <v>1</v>
+      </c>
+      <c r="G10" s="4">
+        <v>1377.7362470400001</v>
+      </c>
+      <c r="H10" s="3">
+        <v>3.4448281099250001E-3</v>
+      </c>
+      <c r="I10" s="4">
+        <f t="shared" ref="I10:I16" si="0">G10-G10*(H10)</f>
+        <v>1372.9901824881342</v>
+      </c>
+      <c r="J10" s="3">
+        <v>6</v>
+      </c>
+      <c r="K10" s="25">
+        <v>17</v>
+      </c>
+      <c r="L10" s="5">
+        <f t="shared" ref="L10:L16" si="1">G10-I10</f>
+        <v>4.7460645518658566</v>
+      </c>
+      <c r="M10">
+        <v>6</v>
+      </c>
+      <c r="N10" s="9">
+        <v>1320</v>
+      </c>
+      <c r="O10" s="28">
+        <v>1340</v>
+      </c>
+      <c r="P10">
+        <v>1360</v>
+      </c>
+      <c r="Q10">
+        <v>1380</v>
+      </c>
+      <c r="R10">
+        <v>1400</v>
+      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="G11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="G12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="G13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="G14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="G15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="K15" s="1"/>
-    </row>
-    <row r="16" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="4">
+      <c r="A11" s="13"/>
+      <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3">
         <v>3</v>
       </c>
-      <c r="D17" s="4">
-        <v>4</v>
-      </c>
-      <c r="E17" s="4">
-        <v>1</v>
-      </c>
-      <c r="F17" s="4">
-        <v>0</v>
-      </c>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="14"/>
-      <c r="M17" s="1"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6" t="s">
+      <c r="D11" s="3">
         <v>7</v>
       </c>
-      <c r="C18" s="6">
-        <v>3</v>
-      </c>
-      <c r="D18" s="6">
-        <v>5</v>
-      </c>
-      <c r="E18" s="6">
-        <v>1</v>
-      </c>
-      <c r="F18" s="6">
-        <v>1</v>
-      </c>
-      <c r="G18" s="7">
-        <v>1391.2992307200002</v>
-      </c>
-      <c r="H18" s="6">
-        <v>5.1395017022160001E-3</v>
-      </c>
-      <c r="I18" s="7">
-        <f>G18-G18*(H18)</f>
-        <v>1384.148645955423</v>
-      </c>
-      <c r="J18" s="6">
-        <v>5</v>
-      </c>
-      <c r="K18" s="8">
-        <f>G18-I18</f>
-        <v>7.150584764577161</v>
-      </c>
-      <c r="L18" s="13">
-        <v>17</v>
-      </c>
-      <c r="M18" s="1"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="6">
-        <v>3</v>
-      </c>
-      <c r="D19" s="6">
-        <v>6</v>
-      </c>
-      <c r="E19" s="6">
-        <v>1</v>
-      </c>
-      <c r="F19" s="6">
-        <v>1</v>
-      </c>
-      <c r="G19" s="7">
-        <v>1377.7362470400001</v>
-      </c>
-      <c r="H19" s="6">
-        <v>3.4448281099250001E-3</v>
-      </c>
-      <c r="I19" s="7">
-        <f t="shared" ref="I17:I42" si="0">G19-G19*(H19)</f>
-        <v>1372.9901824881342</v>
-      </c>
-      <c r="J19" s="6">
-        <v>6</v>
-      </c>
-      <c r="K19" s="8">
-        <f t="shared" ref="K17:K35" si="1">G19-I19</f>
-        <v>4.7460645518658566</v>
-      </c>
-      <c r="L19" s="13">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="6">
-        <v>3</v>
-      </c>
-      <c r="D20" s="6">
-        <v>7</v>
-      </c>
-      <c r="E20" s="6">
-        <v>1</v>
-      </c>
-      <c r="F20" s="6">
-        <v>1</v>
-      </c>
-      <c r="G20" s="7">
+      <c r="E11" s="3">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1</v>
+      </c>
+      <c r="G11" s="4">
         <v>1368.8156936548</v>
       </c>
-      <c r="H20" s="6">
+      <c r="H11" s="3">
         <v>9.9303753173170008E-3</v>
       </c>
-      <c r="I20" s="7">
+      <c r="I11" s="4">
         <f t="shared" si="0"/>
         <v>1355.2228400765744</v>
       </c>
-      <c r="J20" s="6">
+      <c r="J11" s="3">
         <v>7</v>
       </c>
-      <c r="K20" s="8">
+      <c r="K11" s="25">
+        <v>17</v>
+      </c>
+      <c r="L11" s="5">
         <f t="shared" si="1"/>
         <v>13.592853578225686</v>
       </c>
-      <c r="L20" s="13">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6" t="s">
+      <c r="M11">
+        <v>7</v>
+      </c>
+      <c r="N11" s="9">
+        <v>1320</v>
+      </c>
+      <c r="O11" s="28">
+        <v>1340</v>
+      </c>
+      <c r="P11">
+        <v>1360</v>
+      </c>
+      <c r="Q11">
+        <v>1380</v>
+      </c>
+      <c r="R11">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" s="13"/>
+      <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C12" s="3">
         <v>3</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D12" s="3">
         <v>8</v>
       </c>
-      <c r="E21" s="6">
-        <v>1</v>
-      </c>
-      <c r="F21" s="6">
-        <v>1</v>
-      </c>
-      <c r="G21" s="7">
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1</v>
+      </c>
+      <c r="G12" s="4">
         <v>1362.4546060800001</v>
       </c>
-      <c r="H21" s="6">
+      <c r="H12" s="3">
         <v>4.8686257382359998E-3</v>
       </c>
-      <c r="I21" s="7">
+      <c r="I12" s="4">
         <f t="shared" si="0"/>
         <v>1355.8213245176607</v>
       </c>
-      <c r="J21" s="6">
+      <c r="J12" s="3">
         <v>8</v>
       </c>
-      <c r="K21" s="8">
+      <c r="K12" s="25">
+        <v>17</v>
+      </c>
+      <c r="L12" s="5">
         <f t="shared" si="1"/>
         <v>6.6332815623393344</v>
       </c>
-      <c r="L21" s="13">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6" t="s">
+      <c r="M12">
+        <v>8</v>
+      </c>
+      <c r="N12" s="9">
+        <v>1320</v>
+      </c>
+      <c r="O12" s="28">
+        <v>1340</v>
+      </c>
+      <c r="P12">
+        <v>1360</v>
+      </c>
+      <c r="Q12">
+        <v>1380</v>
+      </c>
+      <c r="R12">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="13"/>
+      <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C13" s="3">
         <v>3</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D13" s="3">
         <v>9</v>
       </c>
-      <c r="E22" s="6">
-        <v>1</v>
-      </c>
-      <c r="F22" s="6">
-        <v>1</v>
-      </c>
-      <c r="G22" s="7">
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1</v>
+      </c>
+      <c r="G13" s="4">
         <v>1358.1207552000001</v>
       </c>
-      <c r="H22" s="6">
+      <c r="H13" s="3">
         <v>9.05695157865E-3</v>
       </c>
-      <c r="I22" s="7">
+      <c r="I13" s="4">
         <f t="shared" si="0"/>
         <v>1345.8203212821941</v>
       </c>
-      <c r="J22" s="6">
+      <c r="J13" s="3">
         <v>9</v>
       </c>
-      <c r="K22" s="8">
+      <c r="K13" s="25">
+        <v>17</v>
+      </c>
+      <c r="L13" s="5">
         <f t="shared" si="1"/>
         <v>12.300433917806004</v>
       </c>
-      <c r="L22" s="13">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6" t="s">
+      <c r="M13">
+        <v>9</v>
+      </c>
+      <c r="N13" s="9">
+        <v>1320</v>
+      </c>
+      <c r="O13" s="28">
+        <v>1340</v>
+      </c>
+      <c r="P13">
+        <v>1360</v>
+      </c>
+      <c r="Q13">
+        <v>1380</v>
+      </c>
+      <c r="R13">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" s="13"/>
+      <c r="B14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C14" s="3">
         <v>3</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D14" s="3">
         <v>10</v>
       </c>
-      <c r="E23" s="6">
-        <v>1</v>
-      </c>
-      <c r="F23" s="6">
-        <v>1</v>
-      </c>
-      <c r="G23" s="7">
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
+      <c r="G14" s="4">
         <v>1353.4088811619201</v>
       </c>
-      <c r="H23" s="6">
+      <c r="H14" s="3">
         <v>9.1839999999999995E-3</v>
       </c>
-      <c r="I23" s="7">
+      <c r="I14" s="4">
         <f t="shared" si="0"/>
         <v>1340.9791739973291</v>
       </c>
-      <c r="J23" s="6">
+      <c r="J14" s="3">
         <v>10</v>
       </c>
-      <c r="K23" s="8">
+      <c r="K14" s="25">
+        <v>17</v>
+      </c>
+      <c r="L14" s="5">
         <f t="shared" si="1"/>
         <v>12.429707164591036</v>
       </c>
-      <c r="L23" s="13">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="5"/>
-      <c r="B24" s="6" t="s">
+      <c r="M14">
+        <v>10</v>
+      </c>
+      <c r="N14" s="9">
+        <v>1320</v>
+      </c>
+      <c r="O14" s="28">
+        <v>1340</v>
+      </c>
+      <c r="P14">
+        <v>1360</v>
+      </c>
+      <c r="Q14">
+        <v>1380</v>
+      </c>
+      <c r="R14">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="13"/>
+      <c r="B15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C15" s="3">
         <v>3</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D15" s="3">
         <v>11</v>
       </c>
-      <c r="E24" s="6">
-        <v>1</v>
-      </c>
-      <c r="F24" s="6">
-        <v>1</v>
-      </c>
-      <c r="G24" s="7">
+      <c r="E15" s="3">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
+      <c r="G15" s="4">
         <v>1353.40888697738</v>
       </c>
-      <c r="H24" s="6">
+      <c r="H15" s="3">
         <v>8.8209708334200006E-3</v>
       </c>
-      <c r="I24" s="7">
+      <c r="I15" s="4">
         <f t="shared" si="0"/>
         <v>1341.4705066596612</v>
       </c>
-      <c r="J24" s="6">
+      <c r="J15" s="3">
         <v>10</v>
       </c>
-      <c r="K24" s="8">
+      <c r="K15" s="25">
+        <v>17</v>
+      </c>
+      <c r="L15" s="5">
         <f t="shared" si="1"/>
         <v>11.938380317718838</v>
       </c>
-      <c r="L24" s="13">
+      <c r="M15">
+        <v>11</v>
+      </c>
+      <c r="N15" s="9">
+        <v>1320</v>
+      </c>
+      <c r="O15" s="28">
+        <v>1340</v>
+      </c>
+      <c r="P15">
+        <v>1360</v>
+      </c>
+      <c r="Q15">
+        <v>1380</v>
+      </c>
+      <c r="R15">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="14"/>
+      <c r="B16" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="9"/>
-      <c r="B25" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="10">
+      <c r="C16" s="6">
         <v>3</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D16" s="6">
         <v>12</v>
       </c>
-      <c r="E25" s="10">
-        <v>1</v>
-      </c>
-      <c r="F25" s="10">
-        <v>1</v>
-      </c>
-      <c r="G25" s="11">
+      <c r="E16" s="6">
+        <v>1</v>
+      </c>
+      <c r="F16" s="6">
+        <v>1</v>
+      </c>
+      <c r="G16" s="7">
         <v>1353.4088908800002</v>
       </c>
-      <c r="H25" s="10">
+      <c r="H16" s="6">
         <v>1.0048982073035E-2</v>
       </c>
-      <c r="I25" s="11">
+      <c r="I16" s="7">
         <f t="shared" si="0"/>
         <v>1339.8085091980608</v>
       </c>
-      <c r="J25" s="10">
+      <c r="J16" s="6">
         <v>10</v>
       </c>
-      <c r="K25" s="12">
+      <c r="K16" s="25">
+        <v>17</v>
+      </c>
+      <c r="L16" s="8">
         <f t="shared" si="1"/>
         <v>13.600381681939325</v>
       </c>
-      <c r="L25" s="13">
+      <c r="M16">
+        <v>12</v>
+      </c>
+      <c r="N16" s="9">
+        <v>1320</v>
+      </c>
+      <c r="O16" s="28">
+        <v>1340</v>
+      </c>
+      <c r="P16">
+        <v>1360</v>
+      </c>
+      <c r="Q16">
+        <v>1380</v>
+      </c>
+      <c r="R16">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="2">
+        <v>3</v>
+      </c>
+      <c r="D17" s="2">
+        <v>3</v>
+      </c>
+      <c r="E17" s="15">
+        <v>2</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
+      <c r="G17" s="21"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="23"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="13"/>
+      <c r="B18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="3">
+        <v>3</v>
+      </c>
+      <c r="D18" s="3">
+        <v>4</v>
+      </c>
+      <c r="E18" s="9">
+        <v>2</v>
+      </c>
+      <c r="F18" s="3">
+        <v>1</v>
+      </c>
+      <c r="G18" s="19">
+        <v>1406.3064076799999</v>
+      </c>
+      <c r="H18" s="3">
+        <v>1.93658689376564E-3</v>
+      </c>
+      <c r="I18" s="4">
+        <f>G18-G18*(H18)</f>
+        <v>1403.5829731222682</v>
+      </c>
+      <c r="J18" s="3">
+        <v>4</v>
+      </c>
+      <c r="K18" s="25">
+        <v>25</v>
+      </c>
+      <c r="L18" s="5">
+        <f t="shared" ref="L18:L37" si="2">G18-I18</f>
+        <v>2.7234345577317072</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="13"/>
+      <c r="B19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="3">
+        <v>3</v>
+      </c>
+      <c r="D19" s="3">
+        <v>5</v>
+      </c>
+      <c r="E19" s="9">
+        <v>2</v>
+      </c>
+      <c r="F19" s="3">
+        <v>1</v>
+      </c>
+      <c r="G19" s="19">
+        <v>1389.5306172324099</v>
+      </c>
+      <c r="H19" s="3">
+        <v>8.5295409165939608E-3</v>
+      </c>
+      <c r="I19" s="4">
+        <f>G19-G19*(H19)</f>
+        <v>1377.678558977866</v>
+      </c>
+      <c r="J19" s="3">
+        <v>5</v>
+      </c>
+      <c r="K19" s="25">
+        <v>25</v>
+      </c>
+      <c r="L19" s="5">
+        <f t="shared" si="2"/>
+        <v>11.852058254543863</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="13"/>
+      <c r="B20" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="3">
+        <v>3</v>
+      </c>
+      <c r="D20" s="3">
+        <v>6</v>
+      </c>
+      <c r="E20" s="9">
+        <v>2</v>
+      </c>
+      <c r="F20" s="3">
+        <v>1</v>
+      </c>
+      <c r="G20" s="19">
+        <v>1377.7362470400001</v>
+      </c>
+      <c r="H20" s="3">
+        <v>9.4214521416540707E-3</v>
+      </c>
+      <c r="I20" s="4">
+        <f>G20-G20*(H20)</f>
+        <v>1364.7559709246907</v>
+      </c>
+      <c r="J20" s="3">
+        <v>6</v>
+      </c>
+      <c r="K20" s="25">
+        <v>25</v>
+      </c>
+      <c r="L20" s="5">
+        <f t="shared" si="2"/>
+        <v>12.98027611530938</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="13"/>
+      <c r="B21" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="3">
+        <v>3</v>
+      </c>
+      <c r="D21" s="3">
+        <v>7</v>
+      </c>
+      <c r="E21" s="9">
+        <v>2</v>
+      </c>
+      <c r="F21" s="3">
+        <v>1</v>
+      </c>
+      <c r="G21" s="19">
+        <v>1367.3347238400002</v>
+      </c>
+      <c r="H21" s="3">
+        <v>2.18010300165296E-2</v>
+      </c>
+      <c r="I21" s="4">
+        <f>G21-G21*(H21)</f>
+        <v>1337.5254184829212</v>
+      </c>
+      <c r="J21" s="3">
+        <v>7</v>
+      </c>
+      <c r="K21" s="25">
+        <v>25</v>
+      </c>
+      <c r="L21" s="5">
+        <f t="shared" si="2"/>
+        <v>29.809305357078983</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="13"/>
+      <c r="B22" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="3">
+        <v>3</v>
+      </c>
+      <c r="D22" s="3">
+        <v>8</v>
+      </c>
+      <c r="E22" s="9">
+        <v>2</v>
+      </c>
+      <c r="F22" s="3">
+        <v>1</v>
+      </c>
+      <c r="G22" s="19">
+        <v>1358.17953792</v>
+      </c>
+      <c r="H22" s="3">
+        <v>8.4548217013099298E-3</v>
+      </c>
+      <c r="I22" s="4">
+        <f>G22-G22*(H22)</f>
+        <v>1346.696372088519</v>
+      </c>
+      <c r="J22" s="3">
+        <v>8</v>
+      </c>
+      <c r="K22" s="25">
+        <v>25</v>
+      </c>
+      <c r="L22" s="5">
+        <f t="shared" si="2"/>
+        <v>11.483165831481074</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="13"/>
+      <c r="B23" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="3">
+        <v>3</v>
+      </c>
+      <c r="D23" s="3">
+        <v>9</v>
+      </c>
+      <c r="E23" s="9">
+        <v>2</v>
+      </c>
+      <c r="F23" s="3">
+        <v>1</v>
+      </c>
+      <c r="G23" s="19">
+        <v>1349.2589913600002</v>
+      </c>
+      <c r="H23" s="3">
+        <v>1.15775870202234E-2</v>
+      </c>
+      <c r="I23" s="4">
+        <f>G23-G23*(H23)</f>
+        <v>1333.6378279747109</v>
+      </c>
+      <c r="J23" s="3">
+        <v>9</v>
+      </c>
+      <c r="K23" s="25">
+        <v>25</v>
+      </c>
+      <c r="L23" s="5">
+        <f t="shared" si="2"/>
+        <v>15.621163385289265</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="13"/>
+      <c r="B24" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="3">
+        <v>3</v>
+      </c>
+      <c r="D24" s="3">
+        <v>10</v>
+      </c>
+      <c r="E24" s="9">
+        <v>2</v>
+      </c>
+      <c r="F24" s="3">
+        <v>1</v>
+      </c>
+      <c r="G24" s="19">
+        <v>1342.8591676718199</v>
+      </c>
+      <c r="H24" s="3">
+        <v>0.15880834028830801</v>
+      </c>
+      <c r="I24" s="4">
+        <f>G24-G24*(H24)</f>
+        <v>1129.6019320129194</v>
+      </c>
+      <c r="J24" s="3">
+        <v>10</v>
+      </c>
+      <c r="K24" s="25">
+        <v>25</v>
+      </c>
+      <c r="L24" s="5">
+        <f t="shared" si="2"/>
+        <v>213.25723565890053</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="13"/>
+      <c r="B25" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="3">
+        <v>3</v>
+      </c>
+      <c r="D25" s="3">
+        <v>11</v>
+      </c>
+      <c r="E25" s="9">
+        <v>2</v>
+      </c>
+      <c r="F25" s="3">
+        <v>1</v>
+      </c>
+      <c r="G25" s="19">
+        <v>1336.9486079999999</v>
+      </c>
+      <c r="H25" s="3">
+        <v>0.16017081858058199</v>
+      </c>
+      <c r="I25" s="4">
+        <f>G25-G25*(H25)</f>
+        <v>1122.8084550564704</v>
+      </c>
+      <c r="J25" s="3">
+        <v>11</v>
+      </c>
+      <c r="K25" s="25">
+        <v>25</v>
+      </c>
+      <c r="L25" s="5">
+        <f t="shared" si="2"/>
+        <v>214.14015294352953</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="13"/>
+      <c r="B26" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="3">
+        <v>3</v>
+      </c>
+      <c r="D26" s="3">
+        <v>12</v>
+      </c>
+      <c r="E26" s="9">
+        <v>2</v>
+      </c>
+      <c r="F26" s="3">
+        <v>1</v>
+      </c>
+      <c r="G26" s="19">
+        <v>1332.2367284010299</v>
+      </c>
+      <c r="H26" s="3">
+        <v>8.0312735032272806E-2</v>
+      </c>
+      <c r="I26" s="4">
+        <f>G26-G26*(H26)</f>
+        <v>1225.241153032696</v>
+      </c>
+      <c r="J26" s="3">
+        <v>12</v>
+      </c>
+      <c r="K26" s="25">
+        <v>25</v>
+      </c>
+      <c r="L26" s="5">
+        <f t="shared" si="2"/>
+        <v>106.9955753683339</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="2">
+        <v>4</v>
+      </c>
+      <c r="D27" s="2">
+        <v>2</v>
+      </c>
+      <c r="E27" s="15">
+        <v>1</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0</v>
+      </c>
+      <c r="G27" s="22"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="26">
         <v>17</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="6">
+      <c r="L27" s="23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M27" s="18"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="13"/>
+      <c r="B28" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="9">
+        <v>4</v>
+      </c>
+      <c r="D28" s="9">
         <v>3</v>
       </c>
-      <c r="D26" s="6">
+      <c r="E28" s="9">
+        <v>1</v>
+      </c>
+      <c r="F28" s="3">
+        <v>1</v>
+      </c>
+      <c r="G28" s="4">
+        <v>1492.3079270399999</v>
+      </c>
+      <c r="H28" s="3">
+        <v>3.5548214259258001E-4</v>
+      </c>
+      <c r="I28" s="4">
+        <f>G28-G28*(H28)</f>
+        <v>1491.7774382206878</v>
+      </c>
+      <c r="J28" s="3">
         <v>3</v>
       </c>
-      <c r="E26" s="6">
-        <v>2</v>
-      </c>
-      <c r="F26" s="6">
-        <v>0</v>
-      </c>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="15"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="5"/>
-      <c r="B27" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="6">
-        <v>3</v>
-      </c>
-      <c r="D27" s="6">
+      <c r="K28" s="25">
+        <v>17</v>
+      </c>
+      <c r="L28" s="5">
+        <f t="shared" si="2"/>
+        <v>0.5304888193120405</v>
+      </c>
+      <c r="M28" s="18"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="13"/>
+      <c r="B29" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="9">
         <v>4</v>
       </c>
-      <c r="E27" s="6">
-        <v>2</v>
-      </c>
-      <c r="F27" s="6">
-        <v>1</v>
-      </c>
-      <c r="G27" s="7">
-        <f>1406306.40768/1000</f>
-        <v>1406.3064076799999</v>
-      </c>
-      <c r="H27" s="13">
-        <v>1.9369999999999999E-3</v>
-      </c>
-      <c r="I27" s="7">
-        <f>G27-G27*(H27)</f>
-        <v>1403.5823921683236</v>
-      </c>
-      <c r="J27" s="6">
+      <c r="D29" s="9">
         <v>4</v>
       </c>
-      <c r="K27" s="8">
-        <f>G27-I27</f>
-        <v>2.7240155116762708</v>
-      </c>
-      <c r="L27">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="5"/>
-      <c r="B28" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" s="6">
-        <v>3</v>
-      </c>
-      <c r="D28" s="6">
+      <c r="E29" s="9">
+        <v>1</v>
+      </c>
+      <c r="F29" s="3">
+        <v>1</v>
+      </c>
+      <c r="G29" s="4">
+        <v>1478.29441152</v>
+      </c>
+      <c r="H29" s="3">
+        <v>9.4100162390419392E-3</v>
+      </c>
+      <c r="I29" s="4">
+        <f t="shared" ref="I29:I37" si="3">G29-G29*(H29)</f>
+        <v>1464.3836371015118</v>
+      </c>
+      <c r="J29" s="3">
+        <v>4</v>
+      </c>
+      <c r="K29" s="25">
+        <v>17</v>
+      </c>
+      <c r="L29" s="5">
+        <f t="shared" si="2"/>
+        <v>13.910774418488245</v>
+      </c>
+      <c r="M29" s="18"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" s="13"/>
+      <c r="B30" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="9">
+        <v>4</v>
+      </c>
+      <c r="D30" s="9">
         <v>5</v>
       </c>
-      <c r="E28" s="6">
-        <v>2</v>
-      </c>
-      <c r="F28" s="6">
-        <v>1</v>
-      </c>
-      <c r="G28" s="7">
-        <v>1389.5306172324099</v>
-      </c>
-      <c r="H28" s="6">
-        <v>8.5295409165940007E-3</v>
-      </c>
-      <c r="I28" s="7">
-        <f t="shared" si="0"/>
-        <v>1377.678558977866</v>
-      </c>
-      <c r="J28" s="6">
+      <c r="E30" s="9">
+        <v>1</v>
+      </c>
+      <c r="F30" s="3">
+        <v>1</v>
+      </c>
+      <c r="G30" s="4">
+        <v>1389.5306688000001</v>
+      </c>
+      <c r="H30" s="4">
+        <v>9.6861179604631406E-3</v>
+      </c>
+      <c r="I30" s="4">
+        <f t="shared" si="3"/>
+        <v>1376.071510832322</v>
+      </c>
+      <c r="J30" s="3">
         <v>5</v>
       </c>
-      <c r="K28" s="8">
-        <f t="shared" si="1"/>
-        <v>11.852058254543863</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="5"/>
-      <c r="B29" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C29" s="6">
-        <v>3</v>
-      </c>
-      <c r="D29" s="6">
+      <c r="K30" s="25">
+        <v>17</v>
+      </c>
+      <c r="L30" s="5">
+        <f t="shared" si="2"/>
+        <v>13.459157967678038</v>
+      </c>
+      <c r="M30" s="18"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" s="13"/>
+      <c r="B31" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="9">
+        <v>4</v>
+      </c>
+      <c r="D31" s="9">
         <v>6</v>
       </c>
-      <c r="E29" s="6">
-        <v>2</v>
-      </c>
-      <c r="F29" s="6">
-        <v>1</v>
-      </c>
-      <c r="G29" s="7">
-        <v>1377.7362470400001</v>
-      </c>
-      <c r="H29" s="6">
-        <v>9.4214521416539996E-3</v>
-      </c>
-      <c r="I29" s="7">
-        <f t="shared" si="0"/>
-        <v>1364.7559709246907</v>
-      </c>
-      <c r="J29" s="6">
+      <c r="E31" s="9">
+        <v>1</v>
+      </c>
+      <c r="F31" s="9">
+        <v>1</v>
+      </c>
+      <c r="G31" s="4">
+        <v>1377.73624521228</v>
+      </c>
+      <c r="H31" s="3">
+        <v>9.5640133285550197E-3</v>
+      </c>
+      <c r="I31" s="4">
+        <f t="shared" si="3"/>
+        <v>1364.5595573998364</v>
+      </c>
+      <c r="J31" s="3">
         <v>6</v>
       </c>
-      <c r="K29" s="8">
-        <f t="shared" si="1"/>
-        <v>12.98027611530938</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" s="5"/>
-      <c r="B30" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" s="6">
-        <v>3</v>
-      </c>
-      <c r="D30" s="6">
+      <c r="K31" s="25">
+        <v>17</v>
+      </c>
+      <c r="L31" s="5">
+        <f t="shared" si="2"/>
+        <v>13.176687812443561</v>
+      </c>
+      <c r="M31" s="18"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" s="13"/>
+      <c r="B32" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="9">
+        <v>4</v>
+      </c>
+      <c r="D32" s="9">
         <v>7</v>
       </c>
-      <c r="E30" s="6">
-        <v>2</v>
-      </c>
-      <c r="F30" s="6">
-        <v>1</v>
-      </c>
-      <c r="G30" s="7">
-        <v>1367.3347238400002</v>
-      </c>
-      <c r="H30" s="6">
-        <v>1.6999207381978E-2</v>
-      </c>
-      <c r="I30" s="7">
-        <f t="shared" si="0"/>
-        <v>1344.0911173088643</v>
-      </c>
-      <c r="J30" s="6">
+      <c r="E32" s="9">
+        <v>1</v>
+      </c>
+      <c r="F32" s="9">
+        <v>1</v>
+      </c>
+      <c r="G32" s="4">
+        <v>1368.3651686400001</v>
+      </c>
+      <c r="H32" s="3">
+        <v>6.3571207937942499E-3</v>
+      </c>
+      <c r="I32" s="4">
+        <f t="shared" si="3"/>
+        <v>1359.6663059729349</v>
+      </c>
+      <c r="J32" s="3">
         <v>7</v>
       </c>
-      <c r="K30" s="8">
-        <f t="shared" si="1"/>
-        <v>23.243606531135811</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" s="5"/>
-      <c r="B31" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C31" s="6">
-        <v>3</v>
-      </c>
-      <c r="D31" s="6">
+      <c r="K32" s="25">
+        <v>17</v>
+      </c>
+      <c r="L32" s="5">
+        <f t="shared" si="2"/>
+        <v>8.6988626670652138</v>
+      </c>
+      <c r="M32" s="18"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" s="13"/>
+      <c r="B33" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="9">
+        <v>4</v>
+      </c>
+      <c r="D33" s="9">
         <v>8</v>
       </c>
-      <c r="E31" s="6">
-        <v>2</v>
-      </c>
-      <c r="F31" s="6">
-        <v>1</v>
-      </c>
-      <c r="G31" s="7">
-        <v>1358.179536184</v>
-      </c>
-      <c r="H31" s="6">
-        <v>2.1280000000000001E-3</v>
-      </c>
-      <c r="I31" s="7">
-        <f t="shared" si="0"/>
-        <v>1355.2893301310005</v>
-      </c>
-      <c r="J31" s="6">
+      <c r="E33" s="9">
+        <v>1</v>
+      </c>
+      <c r="F33" s="9">
+        <v>1</v>
+      </c>
+      <c r="G33" s="4">
+        <v>1362.4546060800001</v>
+      </c>
+      <c r="H33" s="3">
+        <v>5.2240339043068901E-3</v>
+      </c>
+      <c r="I33" s="4">
+        <f t="shared" si="3"/>
+        <v>1355.337097024759</v>
+      </c>
+      <c r="J33" s="3">
         <v>8</v>
       </c>
-      <c r="K31" s="8">
-        <f t="shared" si="1"/>
-        <v>2.8902060529994742</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32" s="5"/>
-      <c r="B32" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="6">
-        <v>3</v>
-      </c>
-      <c r="D32" s="6">
+      <c r="K33" s="25">
+        <v>17</v>
+      </c>
+      <c r="L33" s="5">
+        <f t="shared" si="2"/>
+        <v>7.1175090552410438</v>
+      </c>
+      <c r="M33" s="18"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" s="13"/>
+      <c r="B34" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="9">
+        <v>4</v>
+      </c>
+      <c r="D34" s="9">
         <v>9</v>
       </c>
-      <c r="E32" s="6">
-        <v>2</v>
-      </c>
-      <c r="F32" s="6">
-        <v>1</v>
-      </c>
-      <c r="G32" s="7">
-        <v>1349.25898361341</v>
-      </c>
-      <c r="H32" s="6">
-        <v>7.2305171286680004E-3</v>
-      </c>
-      <c r="I32" s="7">
-        <f t="shared" si="0"/>
-        <v>1339.503143421384</v>
-      </c>
-      <c r="J32" s="6">
+      <c r="E34" s="9">
+        <v>1</v>
+      </c>
+      <c r="F34" s="9">
+        <v>1</v>
+      </c>
+      <c r="G34" s="4">
+        <v>1357.7427417599999</v>
+      </c>
+      <c r="H34" s="3">
+        <v>6.6236424533816203E-3</v>
+      </c>
+      <c r="I34" s="4">
+        <f t="shared" si="3"/>
+        <v>1348.7495392949077</v>
+      </c>
+      <c r="J34" s="3">
         <v>9</v>
       </c>
-      <c r="K32" s="8">
-        <f t="shared" si="1"/>
-        <v>9.7558401920259712</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" s="5"/>
-      <c r="B33" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C33" s="6">
-        <v>3</v>
-      </c>
-      <c r="D33" s="6">
+      <c r="K34" s="25">
+        <v>17</v>
+      </c>
+      <c r="L34" s="5">
+        <f t="shared" si="2"/>
+        <v>8.9932024650922813</v>
+      </c>
+      <c r="M34" s="18"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" s="13"/>
+      <c r="B35" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" s="9">
+        <v>4</v>
+      </c>
+      <c r="D35" s="9">
         <v>10</v>
       </c>
-      <c r="E33" s="6">
-        <v>2</v>
-      </c>
-      <c r="F33" s="6">
-        <v>1</v>
-      </c>
-      <c r="G33" s="7">
-        <v>1342.859153914</v>
-      </c>
-      <c r="H33" s="6">
-        <v>8.1440000000000002E-3</v>
-      </c>
-      <c r="I33" s="7">
-        <f t="shared" si="0"/>
-        <v>1331.9229089645244</v>
-      </c>
-      <c r="J33" s="6">
+      <c r="E35" s="9">
+        <v>1</v>
+      </c>
+      <c r="F35" s="9">
+        <v>1</v>
+      </c>
+      <c r="G35" s="4">
+        <v>1353.4088870353</v>
+      </c>
+      <c r="H35" s="3">
+        <v>9.1836175093583401E-3</v>
+      </c>
+      <c r="I35" s="4">
+        <f t="shared" si="3"/>
+        <v>1340.9796974830015</v>
+      </c>
+      <c r="J35" s="3">
         <v>10</v>
       </c>
-      <c r="K33" s="8">
-        <f t="shared" si="1"/>
-        <v>10.936244949475622</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A34" s="5"/>
-      <c r="B34" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" s="6">
-        <v>3</v>
-      </c>
-      <c r="D34" s="6">
+      <c r="K35" s="25">
+        <v>17</v>
+      </c>
+      <c r="L35" s="5">
+        <f t="shared" si="2"/>
+        <v>12.429189552298567</v>
+      </c>
+      <c r="M35" s="18"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" s="13"/>
+      <c r="B36" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" s="3">
+        <v>4</v>
+      </c>
+      <c r="D36" s="3">
         <v>11</v>
       </c>
-      <c r="E34" s="6">
-        <v>2</v>
-      </c>
-      <c r="F34" s="6">
-        <v>1</v>
-      </c>
-      <c r="G34" s="7">
-        <v>1336.94860451</v>
-      </c>
-      <c r="H34" s="6">
-        <v>4.0702115817280596E-3</v>
-      </c>
-      <c r="I34" s="7">
-        <f t="shared" si="0"/>
-        <v>1331.5069408157483</v>
-      </c>
-      <c r="J34" s="6">
-        <v>11</v>
-      </c>
-      <c r="K34" s="8">
-        <f t="shared" si="1"/>
-        <v>5.4416636942517016</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="9"/>
-      <c r="B35" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C35" s="10">
-        <v>3</v>
-      </c>
-      <c r="D35" s="10">
+      <c r="E36" s="9">
+        <v>1</v>
+      </c>
+      <c r="F36" s="3">
+        <v>1</v>
+      </c>
+      <c r="G36" s="4">
+        <v>1353.40888126046</v>
+      </c>
+      <c r="H36" s="3">
+        <v>9.9504740040420002E-3</v>
+      </c>
+      <c r="I36" s="4">
+        <f t="shared" si="3"/>
+        <v>1339.9418213706383</v>
+      </c>
+      <c r="J36" s="3">
+        <v>10</v>
+      </c>
+      <c r="K36" s="25">
+        <v>17</v>
+      </c>
+      <c r="L36" s="5">
+        <f t="shared" si="2"/>
+        <v>13.467059889821712</v>
+      </c>
+      <c r="M36" s="18"/>
+    </row>
+    <row r="37" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="14"/>
+      <c r="B37" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37" s="6">
+        <v>4</v>
+      </c>
+      <c r="D37" s="24">
         <v>12</v>
       </c>
-      <c r="E35" s="10">
-        <v>2</v>
-      </c>
-      <c r="F35" s="10">
-        <v>1</v>
-      </c>
-      <c r="G35" s="11">
-        <v>1332.2367400000001</v>
-      </c>
-      <c r="H35" s="10">
-        <v>6.1147681695967099E-2</v>
-      </c>
-      <c r="I35" s="11">
-        <f t="shared" si="0"/>
-        <v>1250.7735518788072</v>
-      </c>
-      <c r="J35" s="10">
-        <v>12</v>
-      </c>
-      <c r="K35" s="12">
-        <f t="shared" si="1"/>
-        <v>81.463188121192843</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C36">
-        <v>4</v>
-      </c>
-      <c r="D36">
-        <v>0</v>
-      </c>
-      <c r="E36" s="13">
-        <v>1</v>
-      </c>
-      <c r="F36">
-        <v>0</v>
-      </c>
-      <c r="G36" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A37" s="2"/>
-      <c r="C37">
-        <v>4</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37" s="13">
-        <v>1</v>
-      </c>
-      <c r="F37">
-        <v>0</v>
-      </c>
-      <c r="G37" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A38" s="2"/>
-      <c r="C38">
-        <v>4</v>
-      </c>
-      <c r="D38">
-        <v>2</v>
-      </c>
-      <c r="E38" s="13">
-        <v>1</v>
-      </c>
-      <c r="F38">
-        <v>0</v>
-      </c>
-      <c r="G38" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A39" s="2"/>
-      <c r="B39" t="s">
-        <v>31</v>
-      </c>
-      <c r="C39">
-        <v>4</v>
-      </c>
-      <c r="D39">
-        <v>3</v>
-      </c>
-      <c r="E39" s="13">
-        <v>1</v>
-      </c>
-      <c r="F39">
-        <v>1</v>
-      </c>
-      <c r="G39">
-        <f>1491857.39903999/1000</f>
-        <v>1491.85739903999</v>
-      </c>
-      <c r="H39" s="1">
-        <v>5.3598165189285703E-5</v>
-      </c>
-      <c r="I39" s="7">
-        <f t="shared" si="0"/>
-        <v>1491.7774382206774</v>
-      </c>
-      <c r="J39">
-        <v>3</v>
-      </c>
-      <c r="K39" s="1">
-        <f>G39-I39</f>
-        <v>7.9960819312645981E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A40" s="2"/>
-      <c r="B40" t="s">
-        <v>32</v>
-      </c>
-      <c r="C40">
-        <v>4</v>
-      </c>
-      <c r="D40">
-        <v>4</v>
-      </c>
-      <c r="E40" s="13">
-        <v>1</v>
-      </c>
-      <c r="F40" s="13">
-        <v>1</v>
-      </c>
-      <c r="G40">
-        <f>1478294.41131214/1000</f>
-        <v>1478.29441131214</v>
-      </c>
-      <c r="H40">
-        <v>9.0708210911899997E-3</v>
-      </c>
-      <c r="I40" s="7">
-        <f t="shared" si="0"/>
-        <v>1464.8850671870216</v>
-      </c>
-      <c r="J40">
-        <v>4</v>
-      </c>
-      <c r="K40" s="1">
-        <f>G40-I40</f>
-        <v>13.409344125118423</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A41" s="2"/>
-      <c r="B41" t="s">
-        <v>33</v>
-      </c>
-      <c r="C41">
-        <v>4</v>
-      </c>
-      <c r="D41">
-        <v>5</v>
-      </c>
-      <c r="E41" s="13">
-        <v>1</v>
-      </c>
-      <c r="F41" s="13">
-        <v>1</v>
-      </c>
-      <c r="G41">
-        <f>1389530.6688/1000</f>
-        <v>1389.5306688000001</v>
-      </c>
-      <c r="H41">
-        <v>6.4780000000000003E-3</v>
-      </c>
-      <c r="I41" s="7">
-        <f t="shared" si="0"/>
-        <v>1380.5292891275137</v>
-      </c>
-      <c r="J41">
-        <v>5</v>
-      </c>
-      <c r="K41" s="1">
-        <f>G41-I41</f>
-        <v>9.0013796724863369</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A42" s="2"/>
-      <c r="B42" t="s">
-        <v>34</v>
-      </c>
-      <c r="C42">
-        <v>4</v>
-      </c>
-      <c r="D42">
-        <v>6</v>
-      </c>
-      <c r="E42" s="13">
-        <v>1</v>
-      </c>
-      <c r="F42" s="13">
-        <v>1</v>
-      </c>
-      <c r="G42">
-        <f>1377736.24703999/1000</f>
-        <v>1377.7362470399901</v>
-      </c>
-      <c r="H42">
-        <v>9.9143222351309995E-3</v>
-      </c>
-      <c r="I42" s="7">
-        <f t="shared" si="0"/>
-        <v>1364.0769259318156</v>
-      </c>
-      <c r="J42">
-        <v>6</v>
-      </c>
-      <c r="K42" s="1">
-        <f>G42-I42</f>
-        <v>13.659321108174481</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A43" s="2"/>
-      <c r="C43">
-        <v>4</v>
-      </c>
-      <c r="D43">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D44">
-        <v>8</v>
-      </c>
+      <c r="E37" s="24">
+        <v>1</v>
+      </c>
+      <c r="F37" s="6">
+        <v>1</v>
+      </c>
+      <c r="G37" s="7">
+        <v>1353.4088908800002</v>
+      </c>
+      <c r="H37" s="6">
+        <v>9.5510513987088399E-3</v>
+      </c>
+      <c r="I37" s="7">
+        <f t="shared" si="3"/>
+        <v>1340.4824129997357</v>
+      </c>
+      <c r="J37" s="6">
+        <v>10</v>
+      </c>
+      <c r="K37" s="27">
+        <v>17</v>
+      </c>
+      <c r="L37" s="8">
+        <f t="shared" si="2"/>
+        <v>12.926477880264429</v>
+      </c>
+      <c r="M37" s="18"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M38" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A17:A25"/>
-    <mergeCell ref="A7:A14"/>
-    <mergeCell ref="A36:A43"/>
-    <mergeCell ref="A26:A35"/>
+  <mergeCells count="3">
+    <mergeCell ref="A27:A37"/>
+    <mergeCell ref="A8:A16"/>
+    <mergeCell ref="A17:A26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A2506A4-1FD8-4DDF-963A-619A1B7FB958}">
+  <dimension ref="B2:J33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14.77734375" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="21.77734375" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.88671875" customWidth="1"/>
+    <col min="9" max="9" width="21.5546875" customWidth="1"/>
+    <col min="10" max="10" width="21.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C3" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="32"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="11"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" s="33"/>
+      <c r="D7" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7" s="34">
+        <v>-16.775790447589998</v>
+      </c>
+      <c r="H7" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="I7" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="J7" s="37" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" s="34">
+        <v>-13.562983680000116</v>
+      </c>
+      <c r="D8" s="3">
+        <v>32</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F8" s="11">
+        <v>17.7</v>
+      </c>
+      <c r="G8" s="34">
+        <v>-11.794370192409815</v>
+      </c>
+      <c r="H8" s="38">
+        <v>35</v>
+      </c>
+      <c r="I8" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="J8" s="37">
+        <v>15.7</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" s="34">
+        <v>-8.9205533852000372</v>
+      </c>
+      <c r="D9" s="3">
+        <v>30</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F9" s="11">
+        <v>11.6</v>
+      </c>
+      <c r="G9" s="34">
+        <v>-10.401523199999929</v>
+      </c>
+      <c r="H9" s="9">
+        <v>42</v>
+      </c>
+      <c r="I9" s="9">
+        <v>1</v>
+      </c>
+      <c r="J9" s="11">
+        <v>13.3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" s="34">
+        <v>-6.3610875747999671</v>
+      </c>
+      <c r="D10" s="3">
+        <v>17</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F10" s="11">
+        <v>7.7</v>
+      </c>
+      <c r="G10" s="34">
+        <v>-9.1551859200001218</v>
+      </c>
+      <c r="H10" s="9">
+        <v>44</v>
+      </c>
+      <c r="I10" s="9">
+        <v>1</v>
+      </c>
+      <c r="J10" s="11">
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11" s="34">
+        <v>-4.33385088</v>
+      </c>
+      <c r="D11" s="3">
+        <v>16</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F11" s="11">
+        <v>5.6</v>
+      </c>
+      <c r="G11" s="34">
+        <v>-8.9205465599998206</v>
+      </c>
+      <c r="H11" s="9">
+        <v>30</v>
+      </c>
+      <c r="I11" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="J11" s="11">
+        <v>11.6</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12" s="34">
+        <v>-4.7118740380799409</v>
+      </c>
+      <c r="D12" s="3">
+        <v>13</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="F12" s="11">
+        <v>11.48</v>
+      </c>
+      <c r="G12" s="34">
+        <v>-6.3998236881802768</v>
+      </c>
+      <c r="H12" s="9">
+        <v>18</v>
+      </c>
+      <c r="I12" s="9">
+        <v>1</v>
+      </c>
+      <c r="J12" s="11">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13" s="34">
+        <v>5.815459871882922E-6</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="34">
+        <v>-5.9105596718200104</v>
+      </c>
+      <c r="H13" s="9">
+        <v>17</v>
+      </c>
+      <c r="I13" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="J13" s="11">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14" s="35">
+        <v>3.902620164808468E-6</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="35">
+        <v>-4.711879598969972</v>
+      </c>
+      <c r="H14" s="6">
+        <v>19</v>
+      </c>
+      <c r="I14" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="J14" s="39">
+        <v>6.1352000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+    </row>
+    <row r="26" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G26" s="17"/>
+    </row>
+    <row r="27" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G27" s="17"/>
+    </row>
+    <row r="28" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G28" s="17"/>
+    </row>
+    <row r="29" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G29" s="17"/>
+    </row>
+    <row r="30" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G30" s="17"/>
+    </row>
+    <row r="31" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G31" s="17"/>
+    </row>
+    <row r="32" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G32" s="17"/>
+    </row>
+    <row r="33" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G33" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="G3:J3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90CFDD70-E649-48CE-91C3-28276FFEA22B}">
+  <dimension ref="A1:L18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="2">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2">
+        <v>0</v>
+      </c>
+      <c r="G1" s="21"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="10"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="13"/>
+      <c r="B2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="3">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="19">
+        <f>1406306.40768/1000</f>
+        <v>1406.3064076799999</v>
+      </c>
+      <c r="H2" s="9">
+        <v>1.9369999999999999E-3</v>
+      </c>
+      <c r="I2" s="4">
+        <f>G2-G2*(H2)</f>
+        <v>1403.5823921683236</v>
+      </c>
+      <c r="J2" s="3">
+        <v>4</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="5">
+        <f>G2-I2</f>
+        <v>2.7240155116762708</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="13"/>
+      <c r="B3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="3">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="19">
+        <v>1389.5306172324099</v>
+      </c>
+      <c r="H3" s="3">
+        <v>8.5295409165940007E-3</v>
+      </c>
+      <c r="I3" s="4">
+        <f>G3-G3*(H3)</f>
+        <v>1377.678558977866</v>
+      </c>
+      <c r="J3" s="3">
+        <v>5</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="5">
+        <f>G3-I3</f>
+        <v>11.852058254543863</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="13"/>
+      <c r="B4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="3">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3">
+        <v>6</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="19">
+        <v>1377.7362470400001</v>
+      </c>
+      <c r="H4" s="3">
+        <v>9.4214521416539996E-3</v>
+      </c>
+      <c r="I4" s="4">
+        <f>G4-G4*(H4)</f>
+        <v>1364.7559709246907</v>
+      </c>
+      <c r="J4" s="3">
+        <v>6</v>
+      </c>
+      <c r="K4" s="3"/>
+      <c r="L4" s="5">
+        <f>G4-I4</f>
+        <v>12.98027611530938</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="13"/>
+      <c r="B5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="3">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3">
+        <v>7</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="19">
+        <v>1367.3347238400002</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1.6999207381978E-2</v>
+      </c>
+      <c r="I5" s="4">
+        <f>G5-G5*(H5)</f>
+        <v>1344.0911173088643</v>
+      </c>
+      <c r="J5" s="3">
+        <v>7</v>
+      </c>
+      <c r="K5" s="3"/>
+      <c r="L5" s="5">
+        <f>G5-I5</f>
+        <v>23.243606531135811</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="13"/>
+      <c r="B6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="3">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3">
+        <v>8</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" s="19">
+        <v>1358.179536184</v>
+      </c>
+      <c r="H6" s="3">
+        <v>2.1280000000000001E-3</v>
+      </c>
+      <c r="I6" s="4">
+        <f>G6-G6*(H6)</f>
+        <v>1355.2893301310005</v>
+      </c>
+      <c r="J6" s="3">
+        <v>8</v>
+      </c>
+      <c r="K6" s="3"/>
+      <c r="L6" s="5">
+        <f>G6-I6</f>
+        <v>2.8902060529994742</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="13"/>
+      <c r="B7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="3">
+        <v>3</v>
+      </c>
+      <c r="D7" s="3">
+        <v>9</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="19">
+        <v>1349.25898361341</v>
+      </c>
+      <c r="H7" s="3">
+        <v>7.2305171286680004E-3</v>
+      </c>
+      <c r="I7" s="4">
+        <f>G7-G7*(H7)</f>
+        <v>1339.503143421384</v>
+      </c>
+      <c r="J7" s="3">
+        <v>9</v>
+      </c>
+      <c r="K7" s="3"/>
+      <c r="L7" s="5">
+        <f>G7-I7</f>
+        <v>9.7558401920259712</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="13"/>
+      <c r="B8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3</v>
+      </c>
+      <c r="D8" s="3">
+        <v>10</v>
+      </c>
+      <c r="E8" s="3">
+        <v>2</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+      <c r="G8" s="19">
+        <v>1342.859153914</v>
+      </c>
+      <c r="H8" s="3">
+        <v>8.1440000000000002E-3</v>
+      </c>
+      <c r="I8" s="4">
+        <f>G8-G8*(H8)</f>
+        <v>1331.9229089645244</v>
+      </c>
+      <c r="J8" s="3">
+        <v>10</v>
+      </c>
+      <c r="K8" s="3"/>
+      <c r="L8" s="5">
+        <f>G8-I8</f>
+        <v>10.936244949475622</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="13"/>
+      <c r="B9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="3">
+        <v>3</v>
+      </c>
+      <c r="D9" s="3">
+        <v>11</v>
+      </c>
+      <c r="E9" s="3">
+        <v>2</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1</v>
+      </c>
+      <c r="G9" s="19">
+        <v>1336.94860451</v>
+      </c>
+      <c r="H9" s="3">
+        <v>4.0702115817280596E-3</v>
+      </c>
+      <c r="I9" s="4">
+        <f>G9-G9*(H9)</f>
+        <v>1331.5069408157483</v>
+      </c>
+      <c r="J9" s="3">
+        <v>11</v>
+      </c>
+      <c r="K9" s="3"/>
+      <c r="L9" s="5">
+        <f>G9-I9</f>
+        <v>5.4416636942517016</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="14"/>
+      <c r="B10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="6">
+        <v>3</v>
+      </c>
+      <c r="D10" s="6">
+        <v>12</v>
+      </c>
+      <c r="E10" s="6">
+        <v>2</v>
+      </c>
+      <c r="F10" s="6">
+        <v>1</v>
+      </c>
+      <c r="G10" s="20">
+        <v>1332.2367400000001</v>
+      </c>
+      <c r="H10" s="6">
+        <v>6.1147681695967099E-2</v>
+      </c>
+      <c r="I10" s="7">
+        <f>G10-G10*(H10)</f>
+        <v>1250.7735518788072</v>
+      </c>
+      <c r="J10" s="6">
+        <v>12</v>
+      </c>
+      <c r="K10" s="6"/>
+      <c r="L10" s="8">
+        <f>G10-I10</f>
+        <v>81.463188121192843</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2">
+        <v>4</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="15">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="10"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="13"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3">
+        <v>4</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
+      <c r="E12" s="9">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="11"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="13"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3">
+        <v>4</v>
+      </c>
+      <c r="D13" s="3">
+        <v>2</v>
+      </c>
+      <c r="E13" s="9">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="11"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="13"/>
+      <c r="B14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="3">
+        <v>4</v>
+      </c>
+      <c r="D14" s="3">
+        <v>3</v>
+      </c>
+      <c r="E14" s="9">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
+      <c r="G14" s="3">
+        <f>1491857.39903999/1000</f>
+        <v>1491.85739903999</v>
+      </c>
+      <c r="H14" s="4">
+        <v>5.3598165189285703E-5</v>
+      </c>
+      <c r="I14" s="4">
+        <f>G14-G14*(H14)</f>
+        <v>1491.7774382206774</v>
+      </c>
+      <c r="J14" s="3">
+        <v>3</v>
+      </c>
+      <c r="K14" s="3"/>
+      <c r="L14" s="5">
+        <f>G14-I14</f>
+        <v>7.9960819312645981E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="13"/>
+      <c r="B15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="3">
+        <v>4</v>
+      </c>
+      <c r="D15" s="3">
+        <v>4</v>
+      </c>
+      <c r="E15" s="9">
+        <v>1</v>
+      </c>
+      <c r="F15" s="9">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3">
+        <f>1478294.41131214/1000</f>
+        <v>1478.29441131214</v>
+      </c>
+      <c r="H15" s="3">
+        <v>9.0708210911899997E-3</v>
+      </c>
+      <c r="I15" s="4">
+        <f>G15-G15*(H15)</f>
+        <v>1464.8850671870216</v>
+      </c>
+      <c r="J15" s="3">
+        <v>4</v>
+      </c>
+      <c r="K15" s="3"/>
+      <c r="L15" s="5">
+        <f>G15-I15</f>
+        <v>13.409344125118423</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="13"/>
+      <c r="B16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="3">
+        <v>4</v>
+      </c>
+      <c r="D16" s="3">
+        <v>5</v>
+      </c>
+      <c r="E16" s="9">
+        <v>1</v>
+      </c>
+      <c r="F16" s="9">
+        <v>1</v>
+      </c>
+      <c r="G16" s="3">
+        <f>1389530.6688/1000</f>
+        <v>1389.5306688000001</v>
+      </c>
+      <c r="H16" s="3">
+        <v>6.4780000000000003E-3</v>
+      </c>
+      <c r="I16" s="4">
+        <f>G16-G16*(H16)</f>
+        <v>1380.5292891275137</v>
+      </c>
+      <c r="J16" s="3">
+        <v>5</v>
+      </c>
+      <c r="K16" s="3"/>
+      <c r="L16" s="5">
+        <f>G16-I16</f>
+        <v>9.0013796724863369</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="13"/>
+      <c r="B17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="3">
+        <v>4</v>
+      </c>
+      <c r="D17" s="3">
+        <v>6</v>
+      </c>
+      <c r="E17" s="9">
+        <v>1</v>
+      </c>
+      <c r="F17" s="9">
+        <v>1</v>
+      </c>
+      <c r="G17" s="3">
+        <f>1377736.24703999/1000</f>
+        <v>1377.7362470399901</v>
+      </c>
+      <c r="H17" s="3">
+        <v>9.9143222351309995E-3</v>
+      </c>
+      <c r="I17" s="4">
+        <f>G17-G17*(H17)</f>
+        <v>1364.0769259318156</v>
+      </c>
+      <c r="J17" s="3">
+        <v>6</v>
+      </c>
+      <c r="K17" s="3"/>
+      <c r="L17" s="5">
+        <f>G17-I17</f>
+        <v>13.659321108174481</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="14"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6">
+        <v>4</v>
+      </c>
+      <c r="D18" s="6">
+        <v>7</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A10"/>
+    <mergeCell ref="A11:A18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
report and testbench update
</commit_message>
<xml_diff>
--- a/src/testbench.xlsx
+++ b/src/testbench.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Semester_project_git\2022-msc-sem-proj-nseemann\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598DB709-51D0-4520-B383-2230C4CB07C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF99B4D2-ACB0-4B4D-B3D4-5D3BA56026F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5F350800-DD2F-4C68-9341-F5452F06AE8A}"/>
+    <workbookView xWindow="17148" yWindow="7212" windowWidth="23040" windowHeight="6120" xr2:uid="{5F350800-DD2F-4C68-9341-F5452F06AE8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="81">
   <si>
     <t>default params</t>
   </si>
@@ -272,10 +272,13 @@
     <t>17.7,17.1</t>
   </si>
   <si>
-    <t>rounds</t>
-  </si>
-  <si>
     <t>distance costs/period operating</t>
+  </si>
+  <si>
+    <t>sum(numV_D)</t>
+  </si>
+  <si>
+    <t>utilization</t>
   </si>
 </sst>
 </file>
@@ -395,7 +398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -411,7 +414,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -454,6 +456,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1097,7 +1101,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$9:$Q$16</c:f>
+              <c:f>Sheet1!$R$9:$R$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1157,7 +1161,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$R$9:$R$16</c:f>
+              <c:f>Sheet1!$S$9:$S$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1217,7 +1221,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$S$9:$S$16</c:f>
+              <c:f>Sheet1!$T$9:$T$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1277,7 +1281,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$9:$T$16</c:f>
+              <c:f>Sheet1!$U$9:$U$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1337,7 +1341,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$U$9:$U$16</c:f>
+              <c:f>Sheet1!$V$9:$V$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1749,7 +1753,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$9:$N$16</c:f>
+              <c:f>Sheet1!$O$9:$O$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1971,37 +1975,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-CH"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -2022,9 +1996,45 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$J$18:$J$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$18:$N$26</c:f>
+              <c:f>Sheet1!$O$18:$O$26</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2084,6 +2094,62 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Total added skips</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-CH"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2148,7 +2214,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Weekly</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> average cost per period (x1000 MWK)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-CH"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3894,13 +4020,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>974270</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>43543</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>426538</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>155183</xdr:rowOff>
@@ -3932,13 +4058,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>28</xdr:col>
+      <xdr:col>29</xdr:col>
       <xdr:colOff>555171</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>76199</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>36</xdr:col>
+      <xdr:col>37</xdr:col>
       <xdr:colOff>250371</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>32656</xdr:rowOff>
@@ -3969,15 +4095,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>468086</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>391885</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>130629</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>163286</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>130629</xdr:rowOff>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>566056</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>141514</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4302,10 +4428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82F78E04-2C07-4460-BA33-A46D4195128A}">
-  <dimension ref="A1:U38"/>
+  <dimension ref="A1:V37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AO17" sqref="AO17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4313,19 +4439,20 @@
     <col min="1" max="1" width="16.6640625" customWidth="1"/>
     <col min="2" max="2" width="21.21875" customWidth="1"/>
     <col min="7" max="7" width="16.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" customWidth="1"/>
     <col min="9" max="9" width="10.6640625" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="18.88671875" customWidth="1"/>
-    <col min="12" max="12" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.77734375" customWidth="1"/>
-    <col min="14" max="14" width="21.109375" customWidth="1"/>
-    <col min="16" max="16" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5546875" customWidth="1"/>
-    <col min="18" max="18" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.6640625" customWidth="1"/>
+    <col min="11" max="12" width="18.88671875" customWidth="1"/>
+    <col min="13" max="13" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.21875" customWidth="1"/>
+    <col min="15" max="15" width="21.109375" customWidth="1"/>
+    <col min="17" max="17" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.5546875" customWidth="1"/>
+    <col min="19" max="19" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4360,16 +4487,19 @@
         <v>35</v>
       </c>
       <c r="L1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1" t="s">
         <v>26</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>80</v>
+      </c>
+      <c r="O1" t="s">
         <v>78</v>
       </c>
-      <c r="N1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C2">
         <v>2</v>
       </c>
@@ -4386,7 +4516,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C3">
         <v>2</v>
       </c>
@@ -4403,7 +4533,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C4">
         <v>3</v>
       </c>
@@ -4420,7 +4550,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C5">
         <v>3</v>
       </c>
@@ -4437,7 +4567,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C6">
         <v>3</v>
       </c>
@@ -4454,14 +4584,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A8" s="34" t="s">
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A8" s="33" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -4484,28 +4614,30 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="10"/>
-      <c r="P8">
+      <c r="L8" s="2"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="39"/>
+      <c r="Q8">
         <v>4</v>
       </c>
-      <c r="Q8" s="9">
+      <c r="R8" s="9">
         <v>1320</v>
       </c>
-      <c r="R8" s="25">
+      <c r="S8" s="24">
         <v>1340</v>
       </c>
-      <c r="S8">
+      <c r="T8">
         <v>1360</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <v>1380</v>
       </c>
-      <c r="U8">
+      <c r="V8">
         <v>1400</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A9" s="35"/>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A9" s="34"/>
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
@@ -4534,41 +4666,44 @@
       <c r="J9" s="3">
         <v>5</v>
       </c>
-      <c r="K9" s="22">
+      <c r="K9" s="21">
         <v>17</v>
       </c>
-      <c r="L9" s="5">
+      <c r="L9" s="21">
+        <v>28</v>
+      </c>
+      <c r="M9" s="5">
         <f>G9-I9</f>
         <v>7.150584764577161</v>
       </c>
-      <c r="M9">
-        <v>28</v>
-      </c>
-      <c r="N9" s="1">
+      <c r="N9" s="40">
+        <v>97.438000000000002</v>
+      </c>
+      <c r="O9" s="1">
         <v>41.588999999999999</v>
       </c>
-      <c r="O9" s="1"/>
-      <c r="P9">
+      <c r="P9" s="1"/>
+      <c r="Q9">
         <v>5</v>
       </c>
-      <c r="Q9" s="9">
+      <c r="R9" s="9">
         <v>1320</v>
       </c>
-      <c r="R9" s="25">
+      <c r="S9" s="24">
         <v>1340</v>
       </c>
-      <c r="S9">
+      <c r="T9">
         <v>1360</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <v>1380</v>
       </c>
-      <c r="U9">
+      <c r="V9">
         <v>1400</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A10" s="35"/>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A10" s="34"/>
       <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
@@ -4597,41 +4732,44 @@
       <c r="J10" s="3">
         <v>6</v>
       </c>
-      <c r="K10" s="22">
+      <c r="K10" s="21">
         <v>17</v>
       </c>
-      <c r="L10" s="5">
-        <f t="shared" ref="L10:L16" si="1">G10-I10</f>
+      <c r="L10" s="21">
+        <v>28</v>
+      </c>
+      <c r="M10" s="5">
+        <f t="shared" ref="M10:M16" si="1">G10-I10</f>
         <v>4.7460645518658566</v>
       </c>
-      <c r="M10">
-        <v>28</v>
-      </c>
-      <c r="N10" s="1">
+      <c r="N10" s="40">
+        <v>96.386799999999994</v>
+      </c>
+      <c r="O10" s="1">
         <v>41.104999999999997</v>
       </c>
-      <c r="O10" s="1"/>
-      <c r="P10">
+      <c r="P10" s="1"/>
+      <c r="Q10">
         <v>6</v>
       </c>
-      <c r="Q10" s="9">
+      <c r="R10" s="9">
         <v>1320</v>
       </c>
-      <c r="R10" s="25">
+      <c r="S10" s="24">
         <v>1340</v>
       </c>
-      <c r="S10">
+      <c r="T10">
         <v>1360</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <v>1380</v>
       </c>
-      <c r="U10">
+      <c r="V10">
         <v>1400</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A11" s="35"/>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A11" s="34"/>
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
@@ -4660,41 +4798,44 @@
       <c r="J11" s="3">
         <v>7</v>
       </c>
-      <c r="K11" s="22">
+      <c r="K11" s="21">
         <v>17</v>
       </c>
-      <c r="L11" s="5">
+      <c r="L11" s="21">
+        <v>28</v>
+      </c>
+      <c r="M11" s="5">
         <f t="shared" si="1"/>
         <v>13.592853578225686</v>
       </c>
-      <c r="M11">
-        <v>28</v>
-      </c>
-      <c r="N11" s="1">
+      <c r="N11" s="40">
+        <v>95.695400000000006</v>
+      </c>
+      <c r="O11" s="1">
         <v>40.786000000000001</v>
       </c>
-      <c r="O11" s="1"/>
-      <c r="P11">
+      <c r="P11" s="1"/>
+      <c r="Q11">
         <v>7</v>
       </c>
-      <c r="Q11" s="9">
+      <c r="R11" s="9">
         <v>1320</v>
       </c>
-      <c r="R11" s="25">
+      <c r="S11" s="24">
         <v>1340</v>
       </c>
-      <c r="S11">
+      <c r="T11">
         <v>1360</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <v>1380</v>
       </c>
-      <c r="U11">
+      <c r="V11">
         <v>1400</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A12" s="35"/>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A12" s="34"/>
       <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
@@ -4723,41 +4864,44 @@
       <c r="J12" s="3">
         <v>8</v>
       </c>
-      <c r="K12" s="22">
+      <c r="K12" s="21">
         <v>17</v>
       </c>
-      <c r="L12" s="5">
+      <c r="L12" s="21">
+        <v>27</v>
+      </c>
+      <c r="M12" s="5">
         <f t="shared" si="1"/>
         <v>6.6332815623393344</v>
       </c>
-      <c r="M12">
-        <v>27</v>
-      </c>
-      <c r="N12" s="1">
+      <c r="N12" s="40">
+        <v>98.728399999999993</v>
+      </c>
+      <c r="O12" s="1">
         <v>42.061</v>
       </c>
-      <c r="O12" s="1"/>
-      <c r="P12">
+      <c r="P12" s="1"/>
+      <c r="Q12">
         <v>8</v>
       </c>
-      <c r="Q12" s="9">
+      <c r="R12" s="9">
         <v>1320</v>
       </c>
-      <c r="R12" s="25">
+      <c r="S12" s="24">
         <v>1340</v>
       </c>
-      <c r="S12">
+      <c r="T12">
         <v>1360</v>
       </c>
-      <c r="T12">
+      <c r="U12">
         <v>1380</v>
       </c>
-      <c r="U12">
+      <c r="V12">
         <v>1400</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A13" s="35"/>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A13" s="34"/>
       <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
@@ -4786,41 +4930,44 @@
       <c r="J13" s="3">
         <v>9</v>
       </c>
-      <c r="K13" s="22">
+      <c r="K13" s="21">
         <v>17</v>
       </c>
-      <c r="L13" s="5">
+      <c r="L13" s="21">
+        <v>27</v>
+      </c>
+      <c r="M13" s="5">
         <f t="shared" si="1"/>
         <v>12.300433917806004</v>
       </c>
-      <c r="M13">
-        <v>27</v>
-      </c>
-      <c r="N13" s="1">
+      <c r="N13" s="40">
+        <v>98.380099999999999</v>
+      </c>
+      <c r="O13" s="1">
         <v>41.901000000000003</v>
       </c>
-      <c r="O13" s="1"/>
-      <c r="P13">
+      <c r="P13" s="1"/>
+      <c r="Q13">
         <v>9</v>
       </c>
-      <c r="Q13" s="9">
+      <c r="R13" s="9">
         <v>1320</v>
       </c>
-      <c r="R13" s="25">
+      <c r="S13" s="24">
         <v>1340</v>
       </c>
-      <c r="S13">
+      <c r="T13">
         <v>1360</v>
       </c>
-      <c r="T13">
+      <c r="U13">
         <v>1380</v>
       </c>
-      <c r="U13">
+      <c r="V13">
         <v>1400</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A14" s="35"/>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A14" s="34"/>
       <c r="B14" s="3" t="s">
         <v>14</v>
       </c>
@@ -4849,41 +4996,44 @@
       <c r="J14" s="3">
         <v>10</v>
       </c>
-      <c r="K14" s="22">
+      <c r="K14" s="21">
         <v>17</v>
       </c>
-      <c r="L14" s="5">
+      <c r="L14" s="21">
+        <v>27</v>
+      </c>
+      <c r="M14" s="5">
         <f t="shared" si="1"/>
         <v>12.429707164591036</v>
       </c>
-      <c r="M14">
-        <v>27</v>
-      </c>
-      <c r="N14" s="1">
+      <c r="N14" s="40">
+        <v>98.001300000000001</v>
+      </c>
+      <c r="O14" s="1">
         <v>41.73</v>
       </c>
-      <c r="O14" s="1"/>
-      <c r="P14">
+      <c r="P14" s="1"/>
+      <c r="Q14">
         <v>10</v>
       </c>
-      <c r="Q14" s="9">
+      <c r="R14" s="9">
         <v>1320</v>
       </c>
-      <c r="R14" s="25">
+      <c r="S14" s="24">
         <v>1340</v>
       </c>
-      <c r="S14">
+      <c r="T14">
         <v>1360</v>
       </c>
-      <c r="T14">
+      <c r="U14">
         <v>1380</v>
       </c>
-      <c r="U14">
+      <c r="V14">
         <v>1400</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A15" s="35"/>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A15" s="34"/>
       <c r="B15" s="3" t="s">
         <v>16</v>
       </c>
@@ -4912,41 +5062,44 @@
       <c r="J15" s="3">
         <v>10</v>
       </c>
-      <c r="K15" s="22">
+      <c r="K15" s="21">
         <v>17</v>
       </c>
-      <c r="L15" s="5">
+      <c r="L15" s="21">
+        <v>27</v>
+      </c>
+      <c r="M15" s="5">
         <f t="shared" si="1"/>
         <v>11.938380317718838</v>
       </c>
-      <c r="M15">
-        <v>27</v>
-      </c>
-      <c r="N15" s="1">
+      <c r="N15" s="40">
+        <v>98.001300000000001</v>
+      </c>
+      <c r="O15" s="1">
         <v>41.725999999999999</v>
       </c>
-      <c r="O15" s="1"/>
-      <c r="P15">
+      <c r="P15" s="1"/>
+      <c r="Q15">
         <v>11</v>
       </c>
-      <c r="Q15" s="9">
+      <c r="R15" s="9">
         <v>1320</v>
       </c>
-      <c r="R15" s="25">
+      <c r="S15" s="24">
         <v>1340</v>
       </c>
-      <c r="S15">
+      <c r="T15">
         <v>1360</v>
       </c>
-      <c r="T15">
+      <c r="U15">
         <v>1380</v>
       </c>
-      <c r="U15">
+      <c r="V15">
         <v>1400</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="36"/>
+    <row r="16" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="35"/>
       <c r="B16" s="6" t="s">
         <v>17</v>
       </c>
@@ -4975,41 +5128,44 @@
       <c r="J16" s="6">
         <v>10</v>
       </c>
-      <c r="K16" s="22">
+      <c r="K16" s="21">
         <v>17</v>
       </c>
-      <c r="L16" s="8">
+      <c r="L16" s="21">
+        <v>27</v>
+      </c>
+      <c r="M16" s="8">
         <f t="shared" si="1"/>
         <v>13.600381681939325</v>
       </c>
-      <c r="M16">
-        <v>27</v>
-      </c>
-      <c r="N16" s="1">
+      <c r="N16" s="40">
+        <v>98.001300000000001</v>
+      </c>
+      <c r="O16" s="1">
         <v>41.725999999999999</v>
       </c>
-      <c r="O16" s="1"/>
-      <c r="P16">
+      <c r="P16" s="1"/>
+      <c r="Q16">
         <v>12</v>
       </c>
-      <c r="Q16" s="9">
+      <c r="R16" s="9">
         <v>1320</v>
       </c>
-      <c r="R16" s="25">
+      <c r="S16" s="24">
         <v>1340</v>
       </c>
-      <c r="S16">
+      <c r="T16">
         <v>1360</v>
       </c>
-      <c r="T16">
+      <c r="U16">
         <v>1380</v>
       </c>
-      <c r="U16">
+      <c r="V16">
         <v>1400</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="34" t="s">
+    <row r="17" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="33" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -5027,16 +5183,18 @@
       <c r="F17" s="2">
         <v>0</v>
       </c>
-      <c r="G17" s="18"/>
+      <c r="G17" s="17"/>
       <c r="H17" s="2"/>
-      <c r="I17" s="19"/>
+      <c r="I17" s="18"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
-      <c r="L17" s="20"/>
-      <c r="O17" s="1"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A18" s="35"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="40"/>
+      <c r="P17" s="1"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" s="34"/>
       <c r="B18" s="3" t="s">
         <v>40</v>
       </c>
@@ -5052,7 +5210,7 @@
       <c r="F18" s="3">
         <v>1</v>
       </c>
-      <c r="G18" s="16">
+      <c r="G18" s="15">
         <v>1406.3064076799999</v>
       </c>
       <c r="H18" s="3">
@@ -5065,23 +5223,26 @@
       <c r="J18" s="3">
         <v>4</v>
       </c>
-      <c r="K18" s="22">
+      <c r="K18" s="21">
         <v>25</v>
       </c>
-      <c r="L18" s="5">
-        <f t="shared" ref="L18:L37" si="3">G18-I18</f>
+      <c r="L18">
+        <v>28</v>
+      </c>
+      <c r="M18" s="5">
+        <f t="shared" ref="M18:M37" si="3">G18-I18</f>
         <v>2.7234345577317072</v>
       </c>
-      <c r="M18">
-        <v>28</v>
-      </c>
-      <c r="N18" s="1">
+      <c r="N18" s="40">
+        <v>98.601100000000002</v>
+      </c>
+      <c r="O18" s="1">
         <v>42.125</v>
       </c>
-      <c r="O18" s="1"/>
-    </row>
-    <row r="19" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="35"/>
+      <c r="P18" s="1"/>
+    </row>
+    <row r="19" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="34"/>
       <c r="B19" s="3" t="s">
         <v>41</v>
       </c>
@@ -5097,7 +5258,7 @@
       <c r="F19" s="3">
         <v>1</v>
       </c>
-      <c r="G19" s="16">
+      <c r="G19" s="15">
         <v>1389.5306172324099</v>
       </c>
       <c r="H19" s="3">
@@ -5110,23 +5271,26 @@
       <c r="J19" s="3">
         <v>5</v>
       </c>
-      <c r="K19" s="22">
+      <c r="K19" s="21">
         <v>25</v>
       </c>
-      <c r="L19" s="5">
+      <c r="L19">
+        <v>28</v>
+      </c>
+      <c r="M19" s="5">
         <f t="shared" si="3"/>
         <v>11.852058254543863</v>
       </c>
-      <c r="M19">
-        <v>28</v>
-      </c>
-      <c r="N19" s="1">
+      <c r="N19" s="40">
+        <v>97.300899999999999</v>
+      </c>
+      <c r="O19" s="1">
         <v>41.526000000000003</v>
       </c>
-      <c r="O19" s="1"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A20" s="35"/>
+      <c r="P19" s="1"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20" s="34"/>
       <c r="B20" s="3" t="s">
         <v>42</v>
       </c>
@@ -5142,7 +5306,7 @@
       <c r="F20" s="3">
         <v>1</v>
       </c>
-      <c r="G20" s="16">
+      <c r="G20" s="15">
         <v>1377.7362470400001</v>
       </c>
       <c r="H20" s="3">
@@ -5155,23 +5319,26 @@
       <c r="J20" s="3">
         <v>6</v>
       </c>
-      <c r="K20" s="22">
+      <c r="K20" s="21">
         <v>25</v>
       </c>
-      <c r="L20" s="5">
+      <c r="L20">
+        <v>28</v>
+      </c>
+      <c r="M20" s="5">
         <f t="shared" si="3"/>
         <v>12.98027611530938</v>
       </c>
-      <c r="M20">
-        <v>28</v>
-      </c>
-      <c r="N20" s="1">
+      <c r="N20" s="40">
+        <v>96.386799999999994</v>
+      </c>
+      <c r="O20" s="1">
         <v>41.104999999999997</v>
       </c>
-      <c r="O20" s="1"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A21" s="35"/>
+      <c r="P20" s="1"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21" s="34"/>
       <c r="B21" s="3" t="s">
         <v>43</v>
       </c>
@@ -5187,7 +5354,7 @@
       <c r="F21" s="3">
         <v>1</v>
       </c>
-      <c r="G21" s="16">
+      <c r="G21" s="15">
         <v>1367.3347238400002</v>
       </c>
       <c r="H21" s="3">
@@ -5200,23 +5367,26 @@
       <c r="J21" s="3">
         <v>7</v>
       </c>
-      <c r="K21" s="22">
+      <c r="K21" s="21">
         <v>25</v>
       </c>
-      <c r="L21" s="5">
+      <c r="L21">
+        <v>27</v>
+      </c>
+      <c r="M21" s="5">
         <f t="shared" si="3"/>
         <v>29.809305357078983</v>
       </c>
-      <c r="M21">
-        <v>27</v>
-      </c>
-      <c r="N21" s="1">
+      <c r="N21" s="40">
+        <v>99.120599999999996</v>
+      </c>
+      <c r="O21" s="1">
         <v>42.241999999999997</v>
       </c>
-      <c r="O21" s="1"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A22" s="35"/>
+      <c r="P21" s="1"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22" s="34"/>
       <c r="B22" s="3" t="s">
         <v>44</v>
       </c>
@@ -5232,7 +5402,7 @@
       <c r="F22" s="3">
         <v>1</v>
       </c>
-      <c r="G22" s="16">
+      <c r="G22" s="15">
         <v>1358.17953792</v>
       </c>
       <c r="H22" s="3">
@@ -5245,23 +5415,26 @@
       <c r="J22" s="3">
         <v>8</v>
       </c>
-      <c r="K22" s="22">
+      <c r="K22" s="21">
         <v>25</v>
       </c>
-      <c r="L22" s="5">
+      <c r="L22">
+        <v>27</v>
+      </c>
+      <c r="M22" s="5">
         <f t="shared" si="3"/>
         <v>11.483165831481074</v>
       </c>
-      <c r="M22">
-        <v>27</v>
-      </c>
-      <c r="N22" s="1">
+      <c r="N22" s="40">
+        <v>98.384799999999998</v>
+      </c>
+      <c r="O22" s="1">
         <v>41.902999999999999</v>
       </c>
-      <c r="O22" s="1"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A23" s="35"/>
+      <c r="P22" s="1"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23" s="34"/>
       <c r="B23" s="3" t="s">
         <v>45</v>
       </c>
@@ -5277,7 +5450,7 @@
       <c r="F23" s="3">
         <v>1</v>
       </c>
-      <c r="G23" s="16">
+      <c r="G23" s="15">
         <v>1349.2589913600002</v>
       </c>
       <c r="H23" s="3">
@@ -5290,23 +5463,26 @@
       <c r="J23" s="3">
         <v>9</v>
       </c>
-      <c r="K23" s="22">
+      <c r="K23" s="21">
         <v>25</v>
       </c>
-      <c r="L23" s="5">
+      <c r="L23">
+        <v>27</v>
+      </c>
+      <c r="M23" s="5">
         <f t="shared" si="3"/>
         <v>15.621163385289265</v>
       </c>
-      <c r="M23">
-        <v>27</v>
-      </c>
-      <c r="N23" s="1">
+      <c r="N23" s="40">
+        <v>97.6678</v>
+      </c>
+      <c r="O23" s="1">
         <v>41.573</v>
       </c>
-      <c r="O23" s="1"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A24" s="35"/>
+      <c r="P23" s="1"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24" s="34"/>
       <c r="B24" s="3" t="s">
         <v>46</v>
       </c>
@@ -5322,7 +5498,7 @@
       <c r="F24" s="3">
         <v>1</v>
       </c>
-      <c r="G24" s="16">
+      <c r="G24" s="15">
         <v>1342.8591676718199</v>
       </c>
       <c r="H24" s="3">
@@ -5335,23 +5511,26 @@
       <c r="J24" s="3">
         <v>10</v>
       </c>
-      <c r="K24" s="22">
+      <c r="K24" s="21">
         <v>25</v>
       </c>
-      <c r="L24" s="5">
+      <c r="L24">
+        <v>27</v>
+      </c>
+      <c r="M24" s="5">
         <f t="shared" si="3"/>
         <v>213.25723565890053</v>
       </c>
-      <c r="M24">
-        <v>27</v>
-      </c>
-      <c r="N24" s="1">
+      <c r="N24" s="40">
+        <v>97.153400000000005</v>
+      </c>
+      <c r="O24" s="1">
         <v>41.335999999999999</v>
       </c>
-      <c r="O24" s="1"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" s="35"/>
+      <c r="P24" s="1"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A25" s="34"/>
       <c r="B25" s="3" t="s">
         <v>47</v>
       </c>
@@ -5367,7 +5546,7 @@
       <c r="F25" s="3">
         <v>1</v>
       </c>
-      <c r="G25" s="16">
+      <c r="G25" s="15">
         <v>1336.9486079999999</v>
       </c>
       <c r="H25" s="3">
@@ -5380,23 +5559,26 @@
       <c r="J25" s="3">
         <v>11</v>
       </c>
-      <c r="K25" s="22">
+      <c r="K25" s="21">
         <v>25</v>
       </c>
-      <c r="L25" s="5">
+      <c r="L25">
+        <v>27</v>
+      </c>
+      <c r="M25" s="5">
         <f t="shared" si="3"/>
         <v>214.14015294352953</v>
       </c>
-      <c r="M25">
-        <v>27</v>
-      </c>
-      <c r="N25" s="1">
+      <c r="N25" s="40">
+        <v>96.678299999999993</v>
+      </c>
+      <c r="O25" s="1">
         <v>41.116999999999997</v>
       </c>
-      <c r="O25" s="1"/>
-    </row>
-    <row r="26" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="35"/>
+      <c r="P25" s="1"/>
+    </row>
+    <row r="26" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="34"/>
       <c r="B26" s="3" t="s">
         <v>48</v>
       </c>
@@ -5412,7 +5594,7 @@
       <c r="F26" s="3">
         <v>1</v>
       </c>
-      <c r="G26" s="16">
+      <c r="G26" s="15">
         <v>1332.2367284010299</v>
       </c>
       <c r="H26" s="3">
@@ -5425,23 +5607,26 @@
       <c r="J26" s="3">
         <v>12</v>
       </c>
-      <c r="K26" s="22">
+      <c r="K26" s="21">
         <v>25</v>
       </c>
-      <c r="L26" s="5">
+      <c r="L26">
+        <v>27</v>
+      </c>
+      <c r="M26" s="5">
         <f t="shared" si="3"/>
         <v>106.9955753683339</v>
       </c>
-      <c r="M26">
-        <v>27</v>
-      </c>
-      <c r="N26" s="1">
+      <c r="N26" s="40">
+        <v>96.299599999999998</v>
+      </c>
+      <c r="O26" s="1">
         <v>40.942</v>
       </c>
-      <c r="O26" s="1"/>
-    </row>
-    <row r="27" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="34" t="s">
+      <c r="P26" s="1"/>
+    </row>
+    <row r="27" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="33" t="s">
         <v>49</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -5459,21 +5644,19 @@
       <c r="F27" s="2">
         <v>0</v>
       </c>
-      <c r="G27" s="19"/>
+      <c r="G27" s="18"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
-      <c r="K27" s="23">
+      <c r="K27" s="22">
         <v>17</v>
       </c>
-      <c r="L27" s="20">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M27" s="15"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A28" s="35"/>
+      <c r="L27" s="22"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="40"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A28" s="34"/>
       <c r="B28" s="3" t="s">
         <v>61</v>
       </c>
@@ -5502,17 +5685,18 @@
       <c r="J28" s="3">
         <v>3</v>
       </c>
-      <c r="K28" s="22">
+      <c r="K28" s="21">
         <v>17</v>
       </c>
-      <c r="L28" s="5">
+      <c r="L28" s="21"/>
+      <c r="M28" s="5">
         <f t="shared" si="3"/>
         <v>0.5304888193120405</v>
       </c>
-      <c r="M28" s="15"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A29" s="35"/>
+      <c r="N28" s="39"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A29" s="34"/>
       <c r="B29" s="3" t="s">
         <v>52</v>
       </c>
@@ -5541,17 +5725,18 @@
       <c r="J29" s="3">
         <v>4</v>
       </c>
-      <c r="K29" s="22">
+      <c r="K29" s="21">
         <v>17</v>
       </c>
-      <c r="L29" s="5">
+      <c r="L29" s="21"/>
+      <c r="M29" s="5">
         <f t="shared" si="3"/>
         <v>13.910774418488245</v>
       </c>
-      <c r="M29" s="15"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A30" s="35"/>
+      <c r="N29" s="39"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A30" s="34"/>
       <c r="B30" s="3" t="s">
         <v>53</v>
       </c>
@@ -5580,17 +5765,18 @@
       <c r="J30" s="3">
         <v>5</v>
       </c>
-      <c r="K30" s="22">
+      <c r="K30" s="21">
         <v>17</v>
       </c>
-      <c r="L30" s="5">
+      <c r="L30" s="21"/>
+      <c r="M30" s="5">
         <f t="shared" si="3"/>
         <v>13.459157967678038</v>
       </c>
-      <c r="M30" s="15"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A31" s="35"/>
+      <c r="N30" s="39"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A31" s="34"/>
       <c r="B31" s="3" t="s">
         <v>54</v>
       </c>
@@ -5619,17 +5805,18 @@
       <c r="J31" s="3">
         <v>6</v>
       </c>
-      <c r="K31" s="22">
+      <c r="K31" s="21">
         <v>17</v>
       </c>
-      <c r="L31" s="5">
+      <c r="L31" s="21"/>
+      <c r="M31" s="5">
         <f t="shared" si="3"/>
         <v>13.176687812443561</v>
       </c>
-      <c r="M31" s="15"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A32" s="35"/>
+      <c r="N31" s="39"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A32" s="34"/>
       <c r="B32" s="3" t="s">
         <v>55</v>
       </c>
@@ -5658,17 +5845,18 @@
       <c r="J32" s="3">
         <v>7</v>
       </c>
-      <c r="K32" s="22">
+      <c r="K32" s="21">
         <v>17</v>
       </c>
-      <c r="L32" s="5">
+      <c r="L32" s="21"/>
+      <c r="M32" s="5">
         <f t="shared" si="3"/>
         <v>8.6988626670652138</v>
       </c>
-      <c r="M32" s="15"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A33" s="35"/>
+      <c r="N32" s="39"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A33" s="34"/>
       <c r="B33" s="3" t="s">
         <v>56</v>
       </c>
@@ -5697,17 +5885,18 @@
       <c r="J33" s="3">
         <v>8</v>
       </c>
-      <c r="K33" s="22">
+      <c r="K33" s="21">
         <v>17</v>
       </c>
-      <c r="L33" s="5">
+      <c r="L33" s="21"/>
+      <c r="M33" s="5">
         <f t="shared" si="3"/>
         <v>7.1175090552410438</v>
       </c>
-      <c r="M33" s="15"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A34" s="35"/>
+      <c r="N33" s="39"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A34" s="34"/>
       <c r="B34" s="3" t="s">
         <v>57</v>
       </c>
@@ -5736,17 +5925,18 @@
       <c r="J34" s="3">
         <v>9</v>
       </c>
-      <c r="K34" s="22">
+      <c r="K34" s="21">
         <v>17</v>
       </c>
-      <c r="L34" s="5">
+      <c r="L34" s="21"/>
+      <c r="M34" s="5">
         <f t="shared" si="3"/>
         <v>8.9932024650922813</v>
       </c>
-      <c r="M34" s="15"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A35" s="35"/>
+      <c r="N34" s="39"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A35" s="34"/>
       <c r="B35" s="3" t="s">
         <v>58</v>
       </c>
@@ -5775,17 +5965,18 @@
       <c r="J35" s="3">
         <v>10</v>
       </c>
-      <c r="K35" s="22">
+      <c r="K35" s="21">
         <v>17</v>
       </c>
-      <c r="L35" s="5">
+      <c r="L35" s="21"/>
+      <c r="M35" s="5">
         <f t="shared" si="3"/>
         <v>12.429189552298567</v>
       </c>
-      <c r="M35" s="15"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A36" s="35"/>
+      <c r="N35" s="39"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A36" s="34"/>
       <c r="B36" s="3" t="s">
         <v>59</v>
       </c>
@@ -5814,27 +6005,28 @@
       <c r="J36" s="3">
         <v>10</v>
       </c>
-      <c r="K36" s="22">
+      <c r="K36" s="21">
         <v>17</v>
       </c>
-      <c r="L36" s="5">
+      <c r="L36" s="21"/>
+      <c r="M36" s="5">
         <f t="shared" si="3"/>
         <v>13.467059889821712</v>
       </c>
-      <c r="M36" s="15"/>
-    </row>
-    <row r="37" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="36"/>
+      <c r="N36" s="39"/>
+    </row>
+    <row r="37" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="35"/>
       <c r="B37" s="6" t="s">
         <v>60</v>
       </c>
       <c r="C37" s="6">
         <v>4</v>
       </c>
-      <c r="D37" s="21">
+      <c r="D37" s="20">
         <v>12</v>
       </c>
-      <c r="E37" s="21">
+      <c r="E37" s="20">
         <v>1</v>
       </c>
       <c r="F37" s="6">
@@ -5853,17 +6045,15 @@
       <c r="J37" s="6">
         <v>10</v>
       </c>
-      <c r="K37" s="24">
+      <c r="K37" s="23">
         <v>17</v>
       </c>
-      <c r="L37" s="8">
+      <c r="L37" s="23"/>
+      <c r="M37" s="8">
         <f t="shared" si="3"/>
         <v>12.926477880264429</v>
       </c>
-      <c r="M37" s="15"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="M38" s="15"/>
+      <c r="N37" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5900,24 +6090,24 @@
   <sheetData>
     <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="37" t="s">
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="39"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="26" t="s">
         <v>65</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -5929,7 +6119,7 @@
       <c r="F4" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="26" t="s">
         <v>65</v>
       </c>
       <c r="H4" s="3" t="s">
@@ -5946,7 +6136,7 @@
       <c r="B5">
         <v>3</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="26" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -5954,7 +6144,7 @@
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="11"/>
-      <c r="G5" s="27" t="s">
+      <c r="G5" s="26" t="s">
         <v>5</v>
       </c>
       <c r="H5" s="3" t="s">
@@ -5967,7 +6157,7 @@
       <c r="B6">
         <v>4</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="26" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -5975,7 +6165,7 @@
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="11"/>
-      <c r="G6" s="27"/>
+      <c r="G6" s="26"/>
       <c r="H6" s="3" t="s">
         <v>72</v>
       </c>
@@ -5990,7 +6180,7 @@
       <c r="B7">
         <v>5</v>
       </c>
-      <c r="C7" s="27"/>
+      <c r="C7" s="26"/>
       <c r="D7" s="3" t="s">
         <v>69</v>
       </c>
@@ -6000,16 +6190,16 @@
       <c r="F7" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="G7" s="28">
+      <c r="G7" s="27">
         <v>-16.775790447589998</v>
       </c>
-      <c r="H7" s="30" t="s">
+      <c r="H7" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="I7" s="30" t="s">
+      <c r="I7" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="J7" s="31" t="s">
+      <c r="J7" s="30" t="s">
         <v>77</v>
       </c>
     </row>
@@ -6017,7 +6207,7 @@
       <c r="B8">
         <v>6</v>
       </c>
-      <c r="C8" s="28">
+      <c r="C8" s="27">
         <v>-13.562983680000116</v>
       </c>
       <c r="D8" s="3">
@@ -6029,16 +6219,16 @@
       <c r="F8" s="11">
         <v>17.7</v>
       </c>
-      <c r="G8" s="28">
+      <c r="G8" s="27">
         <v>-11.794370192409815</v>
       </c>
-      <c r="H8" s="32">
+      <c r="H8" s="31">
         <v>35</v>
       </c>
-      <c r="I8" s="30">
+      <c r="I8" s="29">
         <v>0.5</v>
       </c>
-      <c r="J8" s="31">
+      <c r="J8" s="30">
         <v>15.7</v>
       </c>
     </row>
@@ -6046,7 +6236,7 @@
       <c r="B9">
         <v>7</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="27">
         <v>-8.9205533852000372</v>
       </c>
       <c r="D9" s="3">
@@ -6058,7 +6248,7 @@
       <c r="F9" s="11">
         <v>11.6</v>
       </c>
-      <c r="G9" s="28">
+      <c r="G9" s="27">
         <v>-10.401523199999929</v>
       </c>
       <c r="H9" s="9">
@@ -6075,7 +6265,7 @@
       <c r="B10">
         <v>8</v>
       </c>
-      <c r="C10" s="28">
+      <c r="C10" s="27">
         <v>-6.3610875747999671</v>
       </c>
       <c r="D10" s="3">
@@ -6087,7 +6277,7 @@
       <c r="F10" s="11">
         <v>7.7</v>
       </c>
-      <c r="G10" s="28">
+      <c r="G10" s="27">
         <v>-9.1551859200001218</v>
       </c>
       <c r="H10" s="9">
@@ -6104,7 +6294,7 @@
       <c r="B11">
         <v>9</v>
       </c>
-      <c r="C11" s="28">
+      <c r="C11" s="27">
         <v>-4.33385088</v>
       </c>
       <c r="D11" s="3">
@@ -6116,7 +6306,7 @@
       <c r="F11" s="11">
         <v>5.6</v>
       </c>
-      <c r="G11" s="28">
+      <c r="G11" s="27">
         <v>-8.9205465599998206</v>
       </c>
       <c r="H11" s="9">
@@ -6133,7 +6323,7 @@
       <c r="B12">
         <v>10</v>
       </c>
-      <c r="C12" s="28">
+      <c r="C12" s="27">
         <v>-4.7118740380799409</v>
       </c>
       <c r="D12" s="3">
@@ -6145,7 +6335,7 @@
       <c r="F12" s="11">
         <v>11.48</v>
       </c>
-      <c r="G12" s="28">
+      <c r="G12" s="27">
         <v>-6.3998236881802768</v>
       </c>
       <c r="H12" s="9">
@@ -6162,13 +6352,13 @@
       <c r="B13">
         <v>11</v>
       </c>
-      <c r="C13" s="28">
+      <c r="C13" s="27">
         <v>5.815459871882922E-6</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="11"/>
-      <c r="G13" s="28">
+      <c r="G13" s="27">
         <v>-5.9105596718200104</v>
       </c>
       <c r="H13" s="9">
@@ -6185,13 +6375,13 @@
       <c r="B14">
         <v>12</v>
       </c>
-      <c r="C14" s="29">
+      <c r="C14" s="28">
         <v>3.902620164808468E-6</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="13"/>
-      <c r="G14" s="29">
+      <c r="G14" s="28">
         <v>-4.711879598969972</v>
       </c>
       <c r="H14" s="6">
@@ -6200,13 +6390,13 @@
       <c r="I14" s="6">
         <v>0.5</v>
       </c>
-      <c r="J14" s="33">
+      <c r="J14" s="32">
         <v>6.1352000000000002</v>
       </c>
     </row>
     <row r="22" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
     </row>
     <row r="26" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G26" s="14"/>
@@ -6252,7 +6442,7 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="33" t="s">
         <v>38</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -6270,7 +6460,7 @@
       <c r="F1" s="2">
         <v>0</v>
       </c>
-      <c r="G1" s="18"/>
+      <c r="G1" s="17"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -6278,7 +6468,7 @@
       <c r="L1" s="10"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="35"/>
+      <c r="A2" s="34"/>
       <c r="B2" s="3" t="s">
         <v>32</v>
       </c>
@@ -6294,7 +6484,7 @@
       <c r="F2" s="3">
         <v>1</v>
       </c>
-      <c r="G2" s="16">
+      <c r="G2" s="15">
         <f>1406306.40768/1000</f>
         <v>1406.3064076799999</v>
       </c>
@@ -6315,7 +6505,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="35"/>
+      <c r="A3" s="34"/>
       <c r="B3" s="3" t="s">
         <v>18</v>
       </c>
@@ -6331,7 +6521,7 @@
       <c r="F3" s="3">
         <v>1</v>
       </c>
-      <c r="G3" s="16">
+      <c r="G3" s="15">
         <v>1389.5306172324099</v>
       </c>
       <c r="H3" s="3">
@@ -6351,7 +6541,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="35"/>
+      <c r="A4" s="34"/>
       <c r="B4" s="3" t="s">
         <v>22</v>
       </c>
@@ -6367,7 +6557,7 @@
       <c r="F4" s="3">
         <v>1</v>
       </c>
-      <c r="G4" s="16">
+      <c r="G4" s="15">
         <v>1377.7362470400001</v>
       </c>
       <c r="H4" s="3">
@@ -6387,7 +6577,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="35"/>
+      <c r="A5" s="34"/>
       <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
@@ -6403,7 +6593,7 @@
       <c r="F5" s="3">
         <v>1</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="15">
         <v>1367.3347238400002</v>
       </c>
       <c r="H5" s="3">
@@ -6423,7 +6613,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="35"/>
+      <c r="A6" s="34"/>
       <c r="B6" s="3" t="s">
         <v>24</v>
       </c>
@@ -6439,7 +6629,7 @@
       <c r="F6" s="3">
         <v>1</v>
       </c>
-      <c r="G6" s="16">
+      <c r="G6" s="15">
         <v>1358.179536184</v>
       </c>
       <c r="H6" s="3">
@@ -6459,7 +6649,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="35"/>
+      <c r="A7" s="34"/>
       <c r="B7" s="3" t="s">
         <v>25</v>
       </c>
@@ -6475,7 +6665,7 @@
       <c r="F7" s="3">
         <v>1</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7" s="15">
         <v>1349.25898361341</v>
       </c>
       <c r="H7" s="3">
@@ -6495,7 +6685,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="35"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="3" t="s">
         <v>23</v>
       </c>
@@ -6511,7 +6701,7 @@
       <c r="F8" s="3">
         <v>1</v>
       </c>
-      <c r="G8" s="16">
+      <c r="G8" s="15">
         <v>1342.859153914</v>
       </c>
       <c r="H8" s="3">
@@ -6531,7 +6721,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="35"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
@@ -6547,7 +6737,7 @@
       <c r="F9" s="3">
         <v>1</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9" s="15">
         <v>1336.94860451</v>
       </c>
       <c r="H9" s="3">
@@ -6567,7 +6757,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="36"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="6" t="s">
         <v>20</v>
       </c>
@@ -6583,7 +6773,7 @@
       <c r="F10" s="6">
         <v>1</v>
       </c>
-      <c r="G10" s="17">
+      <c r="G10" s="16">
         <v>1332.2367400000001</v>
       </c>
       <c r="H10" s="6">
@@ -6603,7 +6793,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="33" t="s">
         <v>50</v>
       </c>
       <c r="B11" s="2"/>
@@ -6629,7 +6819,7 @@
       <c r="L11" s="10"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="35"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3">
         <v>4</v>
@@ -6653,7 +6843,7 @@
       <c r="L12" s="11"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="35"/>
+      <c r="A13" s="34"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3">
         <v>4</v>
@@ -6677,7 +6867,7 @@
       <c r="L13" s="11"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="35"/>
+      <c r="A14" s="34"/>
       <c r="B14" s="3" t="s">
         <v>28</v>
       </c>
@@ -6714,7 +6904,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="35"/>
+      <c r="A15" s="34"/>
       <c r="B15" s="3" t="s">
         <v>29</v>
       </c>
@@ -6751,7 +6941,7 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="35"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="3" t="s">
         <v>30</v>
       </c>
@@ -6788,7 +6978,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="35"/>
+      <c r="A17" s="34"/>
       <c r="B17" s="3" t="s">
         <v>31</v>
       </c>
@@ -6825,7 +7015,7 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="36"/>
+      <c r="A18" s="35"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6">
         <v>4</v>

</xml_diff>

<commit_message>
update report uptade some results
</commit_message>
<xml_diff>
--- a/src/testbench.xlsx
+++ b/src/testbench.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Semester_project_git\2022-msc-sem-proj-nseemann\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF99B4D2-ACB0-4B4D-B3D4-5D3BA56026F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E9272A-453B-4754-B6FC-039A257E2A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17148" yWindow="7212" windowWidth="23040" windowHeight="6120" xr2:uid="{5F350800-DD2F-4C68-9341-F5452F06AE8A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5F350800-DD2F-4C68-9341-F5452F06AE8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="84">
   <si>
     <t>default params</t>
   </si>
@@ -279,6 +279,15 @@
   </si>
   <si>
     <t>utilization</t>
+  </si>
+  <si>
+    <t>Composting</t>
+  </si>
+  <si>
+    <t>22-12-05_18-111_output</t>
+  </si>
+  <si>
+    <t>22-12-05_18-301_output</t>
   </si>
 </sst>
 </file>
@@ -398,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -438,6 +447,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -456,8 +467,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4428,10 +4438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82F78E04-2C07-4460-BA33-A46D4195128A}">
-  <dimension ref="A1:V37"/>
+  <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4583,6 +4593,7 @@
       <c r="G6" t="s">
         <v>5</v>
       </c>
+      <c r="N6" s="41"/>
     </row>
     <row r="7" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G7" s="1"/>
@@ -4591,7 +4602,7 @@
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="35" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -4616,7 +4627,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="10"/>
-      <c r="N8" s="39"/>
+      <c r="N8" s="33"/>
       <c r="Q8">
         <v>4</v>
       </c>
@@ -4637,7 +4648,7 @@
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A9" s="34"/>
+      <c r="A9" s="36"/>
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
@@ -4676,7 +4687,7 @@
         <f>G9-I9</f>
         <v>7.150584764577161</v>
       </c>
-      <c r="N9" s="40">
+      <c r="N9" s="34">
         <v>97.438000000000002</v>
       </c>
       <c r="O9" s="1">
@@ -4703,7 +4714,7 @@
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A10" s="34"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
@@ -4742,7 +4753,7 @@
         <f t="shared" ref="M10:M16" si="1">G10-I10</f>
         <v>4.7460645518658566</v>
       </c>
-      <c r="N10" s="40">
+      <c r="N10" s="34">
         <v>96.386799999999994</v>
       </c>
       <c r="O10" s="1">
@@ -4769,7 +4780,7 @@
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A11" s="34"/>
+      <c r="A11" s="36"/>
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
@@ -4808,7 +4819,7 @@
         <f t="shared" si="1"/>
         <v>13.592853578225686</v>
       </c>
-      <c r="N11" s="40">
+      <c r="N11" s="34">
         <v>95.695400000000006</v>
       </c>
       <c r="O11" s="1">
@@ -4835,7 +4846,7 @@
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A12" s="34"/>
+      <c r="A12" s="36"/>
       <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
@@ -4874,7 +4885,7 @@
         <f t="shared" si="1"/>
         <v>6.6332815623393344</v>
       </c>
-      <c r="N12" s="40">
+      <c r="N12" s="34">
         <v>98.728399999999993</v>
       </c>
       <c r="O12" s="1">
@@ -4901,7 +4912,7 @@
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A13" s="34"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
@@ -4940,7 +4951,7 @@
         <f t="shared" si="1"/>
         <v>12.300433917806004</v>
       </c>
-      <c r="N13" s="40">
+      <c r="N13" s="34">
         <v>98.380099999999999</v>
       </c>
       <c r="O13" s="1">
@@ -4967,7 +4978,7 @@
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A14" s="34"/>
+      <c r="A14" s="36"/>
       <c r="B14" s="3" t="s">
         <v>14</v>
       </c>
@@ -5006,7 +5017,7 @@
         <f t="shared" si="1"/>
         <v>12.429707164591036</v>
       </c>
-      <c r="N14" s="40">
+      <c r="N14" s="34">
         <v>98.001300000000001</v>
       </c>
       <c r="O14" s="1">
@@ -5033,7 +5044,7 @@
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A15" s="34"/>
+      <c r="A15" s="36"/>
       <c r="B15" s="3" t="s">
         <v>16</v>
       </c>
@@ -5072,7 +5083,7 @@
         <f t="shared" si="1"/>
         <v>11.938380317718838</v>
       </c>
-      <c r="N15" s="40">
+      <c r="N15" s="34">
         <v>98.001300000000001</v>
       </c>
       <c r="O15" s="1">
@@ -5099,7 +5110,7 @@
       </c>
     </row>
     <row r="16" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="35"/>
+      <c r="A16" s="37"/>
       <c r="B16" s="6" t="s">
         <v>17</v>
       </c>
@@ -5138,7 +5149,7 @@
         <f t="shared" si="1"/>
         <v>13.600381681939325</v>
       </c>
-      <c r="N16" s="40">
+      <c r="N16" s="34">
         <v>98.001300000000001</v>
       </c>
       <c r="O16" s="1">
@@ -5165,7 +5176,7 @@
       </c>
     </row>
     <row r="17" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="35" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -5190,11 +5201,11 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="19"/>
-      <c r="N17" s="40"/>
+      <c r="N17" s="34"/>
       <c r="P17" s="1"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A18" s="34"/>
+      <c r="A18" s="36"/>
       <c r="B18" s="3" t="s">
         <v>40</v>
       </c>
@@ -5233,7 +5244,7 @@
         <f t="shared" ref="M18:M37" si="3">G18-I18</f>
         <v>2.7234345577317072</v>
       </c>
-      <c r="N18" s="40">
+      <c r="N18" s="34">
         <v>98.601100000000002</v>
       </c>
       <c r="O18" s="1">
@@ -5242,7 +5253,7 @@
       <c r="P18" s="1"/>
     </row>
     <row r="19" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="34"/>
+      <c r="A19" s="36"/>
       <c r="B19" s="3" t="s">
         <v>41</v>
       </c>
@@ -5281,7 +5292,7 @@
         <f t="shared" si="3"/>
         <v>11.852058254543863</v>
       </c>
-      <c r="N19" s="40">
+      <c r="N19" s="34">
         <v>97.300899999999999</v>
       </c>
       <c r="O19" s="1">
@@ -5290,7 +5301,7 @@
       <c r="P19" s="1"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A20" s="34"/>
+      <c r="A20" s="36"/>
       <c r="B20" s="3" t="s">
         <v>42</v>
       </c>
@@ -5329,7 +5340,7 @@
         <f t="shared" si="3"/>
         <v>12.98027611530938</v>
       </c>
-      <c r="N20" s="40">
+      <c r="N20" s="34">
         <v>96.386799999999994</v>
       </c>
       <c r="O20" s="1">
@@ -5338,7 +5349,7 @@
       <c r="P20" s="1"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A21" s="34"/>
+      <c r="A21" s="36"/>
       <c r="B21" s="3" t="s">
         <v>43</v>
       </c>
@@ -5377,7 +5388,7 @@
         <f t="shared" si="3"/>
         <v>29.809305357078983</v>
       </c>
-      <c r="N21" s="40">
+      <c r="N21" s="34">
         <v>99.120599999999996</v>
       </c>
       <c r="O21" s="1">
@@ -5386,7 +5397,7 @@
       <c r="P21" s="1"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A22" s="34"/>
+      <c r="A22" s="36"/>
       <c r="B22" s="3" t="s">
         <v>44</v>
       </c>
@@ -5425,7 +5436,7 @@
         <f t="shared" si="3"/>
         <v>11.483165831481074</v>
       </c>
-      <c r="N22" s="40">
+      <c r="N22" s="34">
         <v>98.384799999999998</v>
       </c>
       <c r="O22" s="1">
@@ -5434,7 +5445,7 @@
       <c r="P22" s="1"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A23" s="34"/>
+      <c r="A23" s="36"/>
       <c r="B23" s="3" t="s">
         <v>45</v>
       </c>
@@ -5473,7 +5484,7 @@
         <f t="shared" si="3"/>
         <v>15.621163385289265</v>
       </c>
-      <c r="N23" s="40">
+      <c r="N23" s="34">
         <v>97.6678</v>
       </c>
       <c r="O23" s="1">
@@ -5482,7 +5493,7 @@
       <c r="P23" s="1"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A24" s="34"/>
+      <c r="A24" s="36"/>
       <c r="B24" s="3" t="s">
         <v>46</v>
       </c>
@@ -5521,7 +5532,7 @@
         <f t="shared" si="3"/>
         <v>213.25723565890053</v>
       </c>
-      <c r="N24" s="40">
+      <c r="N24" s="34">
         <v>97.153400000000005</v>
       </c>
       <c r="O24" s="1">
@@ -5530,7 +5541,7 @@
       <c r="P24" s="1"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A25" s="34"/>
+      <c r="A25" s="36"/>
       <c r="B25" s="3" t="s">
         <v>47</v>
       </c>
@@ -5569,7 +5580,7 @@
         <f t="shared" si="3"/>
         <v>214.14015294352953</v>
       </c>
-      <c r="N25" s="40">
+      <c r="N25" s="34">
         <v>96.678299999999993</v>
       </c>
       <c r="O25" s="1">
@@ -5578,7 +5589,7 @@
       <c r="P25" s="1"/>
     </row>
     <row r="26" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="34"/>
+      <c r="A26" s="36"/>
       <c r="B26" s="3" t="s">
         <v>48</v>
       </c>
@@ -5617,7 +5628,7 @@
         <f t="shared" si="3"/>
         <v>106.9955753683339</v>
       </c>
-      <c r="N26" s="40">
+      <c r="N26" s="34">
         <v>96.299599999999998</v>
       </c>
       <c r="O26" s="1">
@@ -5626,7 +5637,7 @@
       <c r="P26" s="1"/>
     </row>
     <row r="27" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="35" t="s">
         <v>49</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -5653,10 +5664,10 @@
       </c>
       <c r="L27" s="22"/>
       <c r="M27" s="19"/>
-      <c r="N27" s="40"/>
+      <c r="N27" s="34"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A28" s="34"/>
+      <c r="A28" s="36"/>
       <c r="B28" s="3" t="s">
         <v>61</v>
       </c>
@@ -5693,10 +5704,10 @@
         <f t="shared" si="3"/>
         <v>0.5304888193120405</v>
       </c>
-      <c r="N28" s="39"/>
+      <c r="N28" s="33"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A29" s="34"/>
+      <c r="A29" s="36"/>
       <c r="B29" s="3" t="s">
         <v>52</v>
       </c>
@@ -5733,10 +5744,10 @@
         <f t="shared" si="3"/>
         <v>13.910774418488245</v>
       </c>
-      <c r="N29" s="39"/>
+      <c r="N29" s="33"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A30" s="34"/>
+      <c r="A30" s="36"/>
       <c r="B30" s="3" t="s">
         <v>53</v>
       </c>
@@ -5773,10 +5784,10 @@
         <f t="shared" si="3"/>
         <v>13.459157967678038</v>
       </c>
-      <c r="N30" s="39"/>
+      <c r="N30" s="33"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A31" s="34"/>
+      <c r="A31" s="36"/>
       <c r="B31" s="3" t="s">
         <v>54</v>
       </c>
@@ -5813,10 +5824,10 @@
         <f t="shared" si="3"/>
         <v>13.176687812443561</v>
       </c>
-      <c r="N31" s="39"/>
+      <c r="N31" s="33"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A32" s="34"/>
+      <c r="A32" s="36"/>
       <c r="B32" s="3" t="s">
         <v>55</v>
       </c>
@@ -5853,10 +5864,10 @@
         <f t="shared" si="3"/>
         <v>8.6988626670652138</v>
       </c>
-      <c r="N32" s="39"/>
+      <c r="N32" s="33"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A33" s="34"/>
+      <c r="A33" s="36"/>
       <c r="B33" s="3" t="s">
         <v>56</v>
       </c>
@@ -5893,10 +5904,10 @@
         <f t="shared" si="3"/>
         <v>7.1175090552410438</v>
       </c>
-      <c r="N33" s="39"/>
+      <c r="N33" s="33"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A34" s="34"/>
+      <c r="A34" s="36"/>
       <c r="B34" s="3" t="s">
         <v>57</v>
       </c>
@@ -5933,10 +5944,10 @@
         <f t="shared" si="3"/>
         <v>8.9932024650922813</v>
       </c>
-      <c r="N34" s="39"/>
+      <c r="N34" s="33"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A35" s="34"/>
+      <c r="A35" s="36"/>
       <c r="B35" s="3" t="s">
         <v>58</v>
       </c>
@@ -5973,10 +5984,10 @@
         <f t="shared" si="3"/>
         <v>12.429189552298567</v>
       </c>
-      <c r="N35" s="39"/>
+      <c r="N35" s="33"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A36" s="34"/>
+      <c r="A36" s="36"/>
       <c r="B36" s="3" t="s">
         <v>59</v>
       </c>
@@ -6013,10 +6024,10 @@
         <f t="shared" si="3"/>
         <v>13.467059889821712</v>
       </c>
-      <c r="N36" s="39"/>
+      <c r="N36" s="33"/>
     </row>
     <row r="37" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="35"/>
+      <c r="A37" s="37"/>
       <c r="B37" s="6" t="s">
         <v>60</v>
       </c>
@@ -6053,7 +6064,93 @@
         <f t="shared" si="3"/>
         <v>12.926477880264429</v>
       </c>
-      <c r="N37" s="39"/>
+      <c r="N37" s="33"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" s="9">
+        <v>3</v>
+      </c>
+      <c r="D38" s="9">
+        <v>3</v>
+      </c>
+      <c r="E38" s="9">
+        <v>1</v>
+      </c>
+      <c r="F38" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" s="9">
+        <v>3</v>
+      </c>
+      <c r="D39" s="9">
+        <v>4</v>
+      </c>
+      <c r="E39" s="9">
+        <v>1</v>
+      </c>
+      <c r="F39" s="9">
+        <v>1</v>
+      </c>
+      <c r="G39" s="1">
+        <v>1298.40367552</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40">
+        <v>3</v>
+      </c>
+      <c r="D40">
+        <v>5</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40" s="1">
+        <f>1283804.03775999/1000</f>
+        <v>1283.80403775999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41">
+        <v>6</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42">
+        <v>7</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6072,7 +6169,7 @@
   <dimension ref="B2:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6090,18 +6187,18 @@
   <sheetData>
     <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="36" t="s">
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="38"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="40"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
@@ -6442,7 +6539,7 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="35" t="s">
         <v>38</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -6468,7 +6565,7 @@
       <c r="L1" s="10"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="34"/>
+      <c r="A2" s="36"/>
       <c r="B2" s="3" t="s">
         <v>32</v>
       </c>
@@ -6505,7 +6602,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="34"/>
+      <c r="A3" s="36"/>
       <c r="B3" s="3" t="s">
         <v>18</v>
       </c>
@@ -6541,7 +6638,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="34"/>
+      <c r="A4" s="36"/>
       <c r="B4" s="3" t="s">
         <v>22</v>
       </c>
@@ -6577,7 +6674,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="34"/>
+      <c r="A5" s="36"/>
       <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
@@ -6613,7 +6710,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="34"/>
+      <c r="A6" s="36"/>
       <c r="B6" s="3" t="s">
         <v>24</v>
       </c>
@@ -6649,7 +6746,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="34"/>
+      <c r="A7" s="36"/>
       <c r="B7" s="3" t="s">
         <v>25</v>
       </c>
@@ -6685,7 +6782,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="34"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="3" t="s">
         <v>23</v>
       </c>
@@ -6721,7 +6818,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="34"/>
+      <c r="A9" s="36"/>
       <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
@@ -6757,7 +6854,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="35"/>
+      <c r="A10" s="37"/>
       <c r="B10" s="6" t="s">
         <v>20</v>
       </c>
@@ -6793,7 +6890,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="35" t="s">
         <v>50</v>
       </c>
       <c r="B11" s="2"/>
@@ -6819,7 +6916,7 @@
       <c r="L11" s="10"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="34"/>
+      <c r="A12" s="36"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3">
         <v>4</v>
@@ -6843,7 +6940,7 @@
       <c r="L12" s="11"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="34"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3">
         <v>4</v>
@@ -6867,7 +6964,7 @@
       <c r="L13" s="11"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="34"/>
+      <c r="A14" s="36"/>
       <c r="B14" s="3" t="s">
         <v>28</v>
       </c>
@@ -6904,7 +7001,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="34"/>
+      <c r="A15" s="36"/>
       <c r="B15" s="3" t="s">
         <v>29</v>
       </c>
@@ -6941,7 +7038,7 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="34"/>
+      <c r="A16" s="36"/>
       <c r="B16" s="3" t="s">
         <v>30</v>
       </c>
@@ -6978,7 +7075,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="34"/>
+      <c r="A17" s="36"/>
       <c r="B17" s="3" t="s">
         <v>31</v>
       </c>
@@ -7015,7 +7112,7 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="35"/>
+      <c r="A18" s="37"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6">
         <v>4</v>

</xml_diff>

<commit_message>
Cleaning up, writing README files
</commit_message>
<xml_diff>
--- a/src/testbench.xlsx
+++ b/src/testbench.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Semester_project_git\2022-msc-sem-proj-nseemann\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EDE859D-31BD-4E36-BE8C-0C6E4A781E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A37EEF-9386-4069-B7EB-01C826A67C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5F350800-DD2F-4C68-9341-F5452F06AE8A}"/>
+    <workbookView xWindow="3348" yWindow="3312" windowWidth="17280" windowHeight="8928" xr2:uid="{5F350800-DD2F-4C68-9341-F5452F06AE8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -306,8 +306,8 @@
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0000E+00"/>
-    <numFmt numFmtId="171" formatCode="0.00000"/>
-    <numFmt numFmtId="173" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -418,7 +418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -461,6 +461,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -479,8 +482,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4453,8 +4454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82F78E04-2C07-4460-BA33-A46D4195128A}">
   <dimension ref="A1:Y45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4625,7 +4626,7 @@
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="39" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -4671,7 +4672,7 @@
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A9" s="37"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
@@ -4716,7 +4717,7 @@
       <c r="O9" s="1">
         <v>41.588999999999999</v>
       </c>
-      <c r="P9" s="43">
+      <c r="P9" s="37">
         <f>Q9/G9</f>
         <v>1.2711956195613217E-3</v>
       </c>
@@ -4746,7 +4747,7 @@
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A10" s="37"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
@@ -4791,7 +4792,7 @@
       <c r="O10" s="1">
         <v>41.104999999999997</v>
       </c>
-      <c r="P10" s="43">
+      <c r="P10" s="37">
         <f t="shared" ref="P10:P15" si="2">Q10/G10</f>
         <v>0</v>
       </c>
@@ -4803,7 +4804,7 @@
         <f>G9-G10</f>
         <v>13.562983680000116</v>
       </c>
-      <c r="S10" s="42">
+      <c r="S10" s="36">
         <f>R10/G9</f>
         <v>9.7484303739471222E-3</v>
       </c>
@@ -4827,7 +4828,7 @@
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A11" s="37"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
@@ -4872,7 +4873,7 @@
       <c r="O11" s="1">
         <v>40.786000000000001</v>
       </c>
-      <c r="P11" s="43">
+      <c r="P11" s="37">
         <f t="shared" si="2"/>
         <v>1.0819351514341825E-3</v>
       </c>
@@ -4884,7 +4885,7 @@
         <f t="shared" ref="R11:R26" si="4">G10-G11</f>
         <v>8.9205533852000372</v>
       </c>
-      <c r="S11" s="42">
+      <c r="S11" s="36">
         <f t="shared" ref="S11:S26" si="5">R11/G10</f>
         <v>6.474790370337876E-3</v>
       </c>
@@ -4908,7 +4909,7 @@
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A12" s="37"/>
+      <c r="A12" s="40"/>
       <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
@@ -4953,7 +4954,7 @@
       <c r="O12" s="1">
         <v>42.061</v>
       </c>
-      <c r="P12" s="43">
+      <c r="P12" s="37">
         <f t="shared" si="2"/>
         <v>3.1377692445109062E-3</v>
       </c>
@@ -4965,7 +4966,7 @@
         <f t="shared" si="4"/>
         <v>6.3610875747999671</v>
       </c>
-      <c r="S12" s="42">
+      <c r="S12" s="36">
         <f t="shared" si="5"/>
         <v>4.6471468761550908E-3</v>
       </c>
@@ -4989,7 +4990,7 @@
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A13" s="37"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
@@ -5034,7 +5035,7 @@
       <c r="O13" s="1">
         <v>41.901000000000003</v>
       </c>
-      <c r="P13" s="43">
+      <c r="P13" s="37">
         <f t="shared" si="2"/>
         <v>6.5250190795404367E-3</v>
       </c>
@@ -5046,7 +5047,7 @@
         <f t="shared" si="4"/>
         <v>4.33385088</v>
       </c>
-      <c r="S13" s="42">
+      <c r="S13" s="36">
         <f t="shared" si="5"/>
         <v>3.1809139626817972E-3</v>
       </c>
@@ -5070,7 +5071,7 @@
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A14" s="37"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="3" t="s">
         <v>14</v>
       </c>
@@ -5115,7 +5116,7 @@
       <c r="O14" s="1">
         <v>41.73</v>
       </c>
-      <c r="P14" s="43">
+      <c r="P14" s="37">
         <f t="shared" si="2"/>
         <v>7.7949196557976835E-3</v>
       </c>
@@ -5127,7 +5128,7 @@
         <f t="shared" si="4"/>
         <v>4.7118740380799409</v>
       </c>
-      <c r="S14" s="42">
+      <c r="S14" s="36">
         <f t="shared" si="5"/>
         <v>3.4694072821131869E-3</v>
       </c>
@@ -5151,7 +5152,7 @@
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A15" s="37"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="3" t="s">
         <v>16</v>
       </c>
@@ -5196,7 +5197,7 @@
       <c r="O15" s="1">
         <v>41.725999999999999</v>
       </c>
-      <c r="P15" s="43">
+      <c r="P15" s="37">
         <f t="shared" si="2"/>
         <v>1.2162088734426341E-2</v>
       </c>
@@ -5208,7 +5209,7 @@
         <f t="shared" si="4"/>
         <v>-5.815459871882922E-6</v>
       </c>
-      <c r="S15" s="42">
+      <c r="S15" s="36">
         <f t="shared" si="5"/>
         <v>-4.2968979684027711E-9</v>
       </c>
@@ -5232,7 +5233,7 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="38"/>
+      <c r="A16" s="41"/>
       <c r="B16" s="6" t="s">
         <v>17</v>
       </c>
@@ -5277,7 +5278,7 @@
       <c r="O16" s="1">
         <v>41.725999999999999</v>
       </c>
-      <c r="P16" s="43">
+      <c r="P16" s="37">
         <f>Q16/G16</f>
         <v>1.5643581641615983E-2</v>
       </c>
@@ -5289,7 +5290,7 @@
         <f t="shared" si="4"/>
         <v>-3.902620164808468E-6</v>
       </c>
-      <c r="S16" s="42">
+      <c r="S16" s="36">
         <f t="shared" si="5"/>
         <v>-2.8835484991711112E-9</v>
       </c>
@@ -5313,7 +5314,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="39" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -5341,10 +5342,10 @@
       <c r="N17" s="34"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
-      <c r="S17" s="42"/>
+      <c r="S17" s="36"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A18" s="37"/>
+      <c r="A18" s="40"/>
       <c r="B18" s="3" t="s">
         <v>40</v>
       </c>
@@ -5392,10 +5393,10 @@
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
-      <c r="S18" s="42"/>
+      <c r="S18" s="36"/>
     </row>
     <row r="19" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="37"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="3" t="s">
         <v>41</v>
       </c>
@@ -5446,13 +5447,13 @@
         <f t="shared" si="4"/>
         <v>16.775790447589998</v>
       </c>
-      <c r="S19" s="42">
+      <c r="S19" s="36">
         <f t="shared" si="5"/>
         <v>1.1928972488481522E-2</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A20" s="37"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="3" t="s">
         <v>42</v>
       </c>
@@ -5503,13 +5504,13 @@
         <f t="shared" si="4"/>
         <v>11.794370192409815</v>
       </c>
-      <c r="S20" s="42">
+      <c r="S20" s="36">
         <f t="shared" si="5"/>
         <v>8.4880246941957914E-3</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A21" s="37"/>
+      <c r="A21" s="40"/>
       <c r="B21" s="3" t="s">
         <v>43</v>
       </c>
@@ -5560,13 +5561,13 @@
         <f t="shared" si="4"/>
         <v>10.401523199999929</v>
       </c>
-      <c r="S21" s="42">
+      <c r="S21" s="36">
         <f t="shared" si="5"/>
         <v>7.5497202184722223E-3</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A22" s="37"/>
+      <c r="A22" s="40"/>
       <c r="B22" s="3" t="s">
         <v>44</v>
       </c>
@@ -5617,13 +5618,13 @@
         <f t="shared" si="4"/>
         <v>9.1551859200001218</v>
       </c>
-      <c r="S22" s="42">
+      <c r="S22" s="36">
         <f t="shared" si="5"/>
         <v>6.6956435468038507E-3</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A23" s="37"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="3" t="s">
         <v>45</v>
       </c>
@@ -5674,13 +5675,13 @@
         <f t="shared" si="4"/>
         <v>8.9205465599998206</v>
       </c>
-      <c r="S23" s="42">
+      <c r="S23" s="36">
         <f t="shared" si="5"/>
         <v>6.5680171957687543E-3</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A24" s="37"/>
+      <c r="A24" s="40"/>
       <c r="B24" s="3" t="s">
         <v>46</v>
       </c>
@@ -5731,13 +5732,13 @@
         <f t="shared" si="4"/>
         <v>6.3998236881802768</v>
       </c>
-      <c r="S24" s="42">
+      <c r="S24" s="36">
         <f t="shared" si="5"/>
         <v>4.7432136670288224E-3</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A25" s="37"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="3" t="s">
         <v>47</v>
       </c>
@@ -5788,13 +5789,13 @@
         <f t="shared" si="4"/>
         <v>5.9105596718200104</v>
       </c>
-      <c r="S25" s="42">
+      <c r="S25" s="36">
         <f t="shared" si="5"/>
         <v>4.4014739699528094E-3</v>
       </c>
     </row>
     <row r="26" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="37"/>
+      <c r="A26" s="40"/>
       <c r="B26" s="3" t="s">
         <v>48</v>
       </c>
@@ -5845,13 +5846,13 @@
         <f t="shared" si="4"/>
         <v>4.711879598969972</v>
       </c>
-      <c r="S26" s="42">
+      <c r="S26" s="36">
         <f t="shared" si="5"/>
         <v>3.524353569595079E-3</v>
       </c>
     </row>
     <row r="27" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="39" t="s">
         <v>49</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -5881,7 +5882,7 @@
       <c r="N27" s="34"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A28" s="37"/>
+      <c r="A28" s="40"/>
       <c r="B28" s="3" t="s">
         <v>61</v>
       </c>
@@ -5921,7 +5922,7 @@
       <c r="N28" s="33"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A29" s="37"/>
+      <c r="A29" s="40"/>
       <c r="B29" s="3" t="s">
         <v>52</v>
       </c>
@@ -5961,7 +5962,7 @@
       <c r="N29" s="33"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A30" s="37"/>
+      <c r="A30" s="40"/>
       <c r="B30" s="3" t="s">
         <v>53</v>
       </c>
@@ -6001,7 +6002,7 @@
       <c r="N30" s="33"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A31" s="37"/>
+      <c r="A31" s="40"/>
       <c r="B31" s="3" t="s">
         <v>54</v>
       </c>
@@ -6041,7 +6042,7 @@
       <c r="N31" s="33"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A32" s="37"/>
+      <c r="A32" s="40"/>
       <c r="B32" s="3" t="s">
         <v>55</v>
       </c>
@@ -6080,8 +6081,8 @@
       </c>
       <c r="N32" s="33"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A33" s="37"/>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A33" s="40"/>
       <c r="B33" s="3" t="s">
         <v>56</v>
       </c>
@@ -6120,8 +6121,8 @@
       </c>
       <c r="N33" s="33"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A34" s="37"/>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A34" s="40"/>
       <c r="B34" s="3" t="s">
         <v>57</v>
       </c>
@@ -6160,8 +6161,8 @@
       </c>
       <c r="N34" s="33"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A35" s="37"/>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A35" s="40"/>
       <c r="B35" s="3" t="s">
         <v>58</v>
       </c>
@@ -6200,8 +6201,8 @@
       </c>
       <c r="N35" s="33"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A36" s="37"/>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A36" s="40"/>
       <c r="B36" s="3" t="s">
         <v>59</v>
       </c>
@@ -6240,8 +6241,8 @@
       </c>
       <c r="N36" s="33"/>
     </row>
-    <row r="37" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="38"/>
+    <row r="37" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="41"/>
       <c r="B37" s="6" t="s">
         <v>60</v>
       </c>
@@ -6279,8 +6280,9 @@
         <v>12.926477880264429</v>
       </c>
       <c r="N37" s="33"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O37" s="38"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>81</v>
       </c>
@@ -6297,7 +6299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>83</v>
       </c>
@@ -6317,7 +6319,7 @@
         <v>1298.40367552</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>82</v>
       </c>
@@ -6337,8 +6339,9 @@
         <f>1283804.03775999/1000</f>
         <v>1283.80403775999</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H40" s="1"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C41">
         <v>2</v>
       </c>
@@ -6352,7 +6355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C42">
         <v>2</v>
       </c>
@@ -6365,9 +6368,13 @@
       <c r="F42">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="J45" s="42">
+      <c r="J42" s="1">
+        <f>(G39-G9)/G9</f>
+        <v>-6.6768925870767978E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J45" s="36">
         <f>((2*G18)-(G39+G18))/(2*G18)</f>
         <v>3.8363877022365468E-2</v>
       </c>
@@ -6407,18 +6414,18 @@
   <sheetData>
     <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="39" t="s">
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="41"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="44"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
@@ -6759,7 +6766,7 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="39" t="s">
         <v>38</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -6785,7 +6792,7 @@
       <c r="L1" s="10"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="37"/>
+      <c r="A2" s="40"/>
       <c r="B2" s="3" t="s">
         <v>32</v>
       </c>
@@ -6822,7 +6829,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="37"/>
+      <c r="A3" s="40"/>
       <c r="B3" s="3" t="s">
         <v>18</v>
       </c>
@@ -6858,7 +6865,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="37"/>
+      <c r="A4" s="40"/>
       <c r="B4" s="3" t="s">
         <v>22</v>
       </c>
@@ -6894,7 +6901,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="37"/>
+      <c r="A5" s="40"/>
       <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
@@ -6930,7 +6937,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="37"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="3" t="s">
         <v>24</v>
       </c>
@@ -6966,7 +6973,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="37"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="3" t="s">
         <v>25</v>
       </c>
@@ -7002,7 +7009,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="37"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="3" t="s">
         <v>23</v>
       </c>
@@ -7038,7 +7045,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="37"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
@@ -7074,7 +7081,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="38"/>
+      <c r="A10" s="41"/>
       <c r="B10" s="6" t="s">
         <v>20</v>
       </c>
@@ -7110,7 +7117,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="39" t="s">
         <v>50</v>
       </c>
       <c r="B11" s="2"/>
@@ -7136,7 +7143,7 @@
       <c r="L11" s="10"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="37"/>
+      <c r="A12" s="40"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3">
         <v>4</v>
@@ -7160,7 +7167,7 @@
       <c r="L12" s="11"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="37"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3">
         <v>4</v>
@@ -7184,7 +7191,7 @@
       <c r="L13" s="11"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="37"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="3" t="s">
         <v>28</v>
       </c>
@@ -7221,7 +7228,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="37"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="3" t="s">
         <v>29</v>
       </c>
@@ -7258,7 +7265,7 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="37"/>
+      <c r="A16" s="40"/>
       <c r="B16" s="3" t="s">
         <v>30</v>
       </c>
@@ -7295,7 +7302,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="37"/>
+      <c r="A17" s="40"/>
       <c r="B17" s="3" t="s">
         <v>31</v>
       </c>
@@ -7332,7 +7339,7 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="38"/>
+      <c r="A18" s="41"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6">
         <v>4</v>

</xml_diff>